<commit_message>
Get daily reddit data: Tue Dec 24 08:10:47 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_12_29.xlsx
+++ b/data/collected_data/2024_12_29.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C520"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,3729 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1hl8stv</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>Holiday mani</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hl8stv</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1hl7rlk</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>Pink christmas bow nails 🎀💕💗</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k56l39b4sq8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1hl4bu2</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>Mini snowglobe turned out better than I thought !</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hl4bu2</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1hl73k9</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>Sugarplum inspired nails!</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hl73k9</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1hl6tkt</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>What all do I need to start making my own press ons?</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hl6tkt/what_all_do_i_need_to_start_making_my_own_press/</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1hl6ij0</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>my first time getting almond!</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hl6ij0</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1hl6auw</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>My First Russian Manicure</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uoq4nxz0bq8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1hl64d1</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How to get this color </t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pba0ehr29q8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1hl62xw</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>How's this for Christmas?</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d8un69pn8q8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1hl5ohq</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>My Christmas nails (took me about an hour to do w/ regular nail polish)</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hl5ohq</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1hl3i4g</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>The art and the inspo! My NYE nails 🛸👾</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d989zkdihp8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1hl3x4w</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t xml:space="preserve">reaction on nails? </t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hl3x4w/reaction_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1hl509n</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>Got my nails done today for the first time in many years</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rlgi3v8wwp8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1hl4p8j</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>😄</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hl4p8j</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1hl4mv6</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>Goldilocks with burgundy polka dots and french manicure</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j5m6ptr0tp8e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1hl4k2x</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>Advice needed new to acrylics-lifting</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hl4k2x/advice_needed_new_to_acrylicslifting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1hl4gq7</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>Love the classic French Tip :)</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hl4gq7</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1hl3ulr</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>What’s the Most Eco-Friendly Nail Trend You’ve Tried?</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hl3ulr/whats_the_most_ecofriendly_nail_trend_youve_tried/</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1hl3pm8</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>my pink &amp; green xmas set!</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hl3pm8</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1hl3oj4</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Finally tried doing a design! </t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hl3oj4</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1hl369y</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t xml:space="preserve">clean goth for christmas! </t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lpkgrah8ep8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1hl30lj</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>❤️✨</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hn2k9e8ocp8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1hl2yht</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Just in time for the holidays 🎄 </t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hl2yht</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1hl2kyz</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>My winter nails</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hl2kyz</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1hl2gx5</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>Christmas Nails! 🎅🏻🎄</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hl2gx5</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1hl25t4</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Went a bit out of my comfort Zone but I love it </t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hl25t4</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1hl24je</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>Hanukkah nails</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fp3upgh04p8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1hl1zfw</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Does the shape fit my fingers or are they too wide/long? </t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9xvdnodp2p8e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1hl1te1</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>Happy holidays</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gec3oxf41p8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1hl1k3x</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>Christmas set 🎄</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vbovq2cmyo8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1hl16p8</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first time getting Christmas nails! What do we think? </t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wxev77z7vo8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1hl13sm</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>Frosted Window First Attempt</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hl13sm</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1hl10z3</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel X Set I did myself for Christmas. Saving cash &amp; getting better at this! </t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dl0wn0rpto8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1hl10dd</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Just for fun. From corpse nails to French.. </t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hl10dd</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1hl0z4c</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>Gold Christmas 🎁 nails</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4yst8xt8to8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1hl0tjv</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>Feel like Lucille from AD</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hl0tjv</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1hl0oln</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>First time doing tips + purple gold festive nails ✨</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hl0oln</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1hl05zv</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>Nail Tech Ate</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9ne4yd9rlo8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1hl04i8</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>December nails</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hl04i8</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1hkzwzo</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>They make absolutely no sense and I love them</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hkzwzo</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1hl037w</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas Set 🎀 </t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2mkkfep2lo8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1hkzlxr</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>opi is actually good??!!!</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hkzlxr/opi_is_actually_good/</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1hkz3d1</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>why do my nails always chip?</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o1bxvz6cco8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1hkz35o</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>did my nails, wanted a little disney</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hkz35o</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1hkyi90</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>Nail tip sizes</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hkyi90</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1hkxh7y</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hand painted Japanese Kintsugi inspired nail art </t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hkxh7y</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1hkxkbg</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>How do I fix this?</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t82pk6t8zn8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1hkxr1w</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How do I take care of my natural nails😭? </t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hkxr1w</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1hkyjkx</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>feeling like myself again 🖤</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4v09bbdo7o8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1hkxbhd</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>couldn't decide on one design for my christmas nails so i just did all of them</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hkxbhd</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1hkx9va</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>First attempt at DIY builder gel</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/epkyhygtwn8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1hkul46</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails keep lifting </t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hkul46/nails_keep_lifting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1hkwrnx</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>Bff gave me a manicure today and I'm so happy!!</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c2rwbjufsn8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1hkwnzr</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>Abalone shell nails</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hkwnzr</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1hkvljr</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time making and wearing press-ons. </t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/on8opm9rin8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1hkw8kv</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first diy Xmas nails 🎄 </t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hkw8kv</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1hkvwt1</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Finally did my nails for Christmas! </t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hkvwt1</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1hkvtrn</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>Get stains off white gel?</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hkvtrn/get_stains_off_white_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1hkurs4</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>Christmas nails 😊</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h29hs8xtbn8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1hkun2b</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>did that😮‍💨</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tppt1lgtan8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1hkulcp</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>Silver Winter</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aexp834fan8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1hkuga8</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>Simple Dark Red</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v3gw88o89n8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1hkuabs</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t xml:space="preserve">It's so natural </t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jz18ykpt7n8e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1hku8es</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>my version of New Year's manicure</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/07m4si1b7n8e1.gif</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1hktybc</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New and old winter nails this season ❄️ 🎅🏻 </t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hktybc</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1hkttmu</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Far from perfect but I like them </t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hhrb85vz3n8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1hktezd</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>why are the whites of my nails doing this? I either have no polish on or the Ohora semi cured strips. They feel strong, gel ruins them. But they get this way sometimes!</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r1xpyroo0n8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1hktq4d</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t xml:space="preserve">When you’re a dark nail girly but it’s Christmas 🖤 ✨ </t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hktq4d</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1hktgdi</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>KBShimmer - Tapped Out</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hktgdi</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1hktdtv</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas spirit </t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ussc4f3f0n8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1hksz6n</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What nail shape would work best with my crooked fingers and curling in nails? </t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9tc8dwd4xm8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1hksyux</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>Holiday 2009 - Barbie serie season 1</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hksyux</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1hksvp9</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas Nails </t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bkq6kuyawm8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1hkss6a</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Holiday nails </t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4fxtkb5jvm8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1hksjh1</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>Nail broke yesterday 😭</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aormumpmtm8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1hks4yl</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>hi guys. 💕❄️✨</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xtlop99fqm8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1hks3eo</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time wearing my natural nails! 🎄 </t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bw4zoxs4qm8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1hks1q9</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>Does anyone know why my nails keep coming off?</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hks1q9/does_anyone_know_why_my_nails_keep_coming_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1hks2j2</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>Quick nude snowy set</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hks2j2</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1hkp56v</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Red/purplish around nail bed </t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/env7mhwj1m8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1hkrigd</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>Damage to nail bed question</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hkrigd/damage_to_nail_bed_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1hknl4y</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>Red band on nails?</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tw14lkzpml8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1hkmc0o</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My nails and my cuticles and the skin around my nails have all like- blended together. </t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hkmc0o/my_nails_and_my_cuticles_and_the_skin_around_my/</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1hki73a</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>Weird Nail Shape?</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/werd9qbmpj8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1hkhalt</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>chemical burn from nail glue?</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hkhalt/chemical_burn_from_nail_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1hkd8nl</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Round or square? </t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hkd8nl</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1hkrwzx</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>My nails for these holidays💅🏻😍🎁</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hkrwzx</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1hkrgck</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Really proud of these! </t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uk1m2n0wkm8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1hkr6qg</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>Xmas Nails 💖🎅🎄</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fss7x27pim8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1hkqmwn</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>Love them 😍</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ch64jp78em8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1hkq0r7</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>just got my nails done and i’m feeling myself 🙆🏻‍♀️💅🏻</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b0ixs1g49m8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1hkptqa</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>Need opinion on the shape</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4mbw65ei7m8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1hkp78l</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>Christmas mani 💅🏼 cute or childish?</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hkp78l</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1hkoi01</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>My last Winter - Christmas themed work for this year. Happy Xmas Everyone!</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a8mdcj8lvl8e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1hko2ti</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails for 8 weeks </t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3a7tu4smrl8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1hknqv5</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>Plaid Christmas French</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h1nv9ifcol8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1hkning</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>What to use for full coverage nails tips?</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hkning/what_to_use_for_full_coverage_nails_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1hknhfe</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>Went for Candy Cane Vibes for Christmas</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ja7tdkunll8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1hkmviv</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>How can I improve my nails appearance?</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hkmviv</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1hkmo4u</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>Grab your shades 🕶 ✨️🎄</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2ilsqazzcl8e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1hl91e4</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Are there colors you don’t have in your polish collection/never wear? </t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hl91e4/are_there_colors_you_dont_have_in_your_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1hl875m</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>Sassy Sauce made me cry...</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p9kzaefdxq8e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1hl7mrl</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>New colour for Xmas tomorrow</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i3m93b7eqq8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1hl7ake</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Finally Tried Birefringence </t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hl7ake</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1hl724g</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>Broken bottle update</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hl724g</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1hl70jr</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Brace for the fallout- a rare polish which suits a difficult christmas </t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9nglj4z2jq8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1hl6ei2</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>Feeling Festive 🎄</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hl6ei2</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1hl662b</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>Mooncat “Lord Vader” x2 magnetized velvet and topped with Glam Polish “Children Can Be Such Monsters” x1</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/iwps02xj9q8e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1hl6149</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Baby laquerista showing off her favourite creations </t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hl6149</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1hl5ohg</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>Mooncat - Forbidden Fruit Velvetized</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hl5ohg</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1hl50aq</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>‘Tis the Season…</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/34anuurlwp8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1hl4qxs</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t xml:space="preserve">When my nails chip, it pulls of the top layer of my actual nail. </t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nlpygkd6up8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1hl4nm1</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>First ilnp order</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b9sykck8tp8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1hl4n5k</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>Finally got House of Hades!</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4819i1w3tp8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1hl4iyo</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>Teal flakie mani</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hl4iyo</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1hl4d6o</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Long time lurker, first time contributor </t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hl4d6o</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1hl4a7l</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>trying to find the perfect pastel glittery holographic (maybe a shimmer) childhood in a bottle pink</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hl4a7l</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1hl3sel</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>dupe for HT menchie cat eye (just the undertone)?</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n852qmxfkp8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1hl3l6w</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>I ordered the Cadillacquer Christmas mystery polishes and got..... nothing</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hl3l6w</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1hl3560</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>Are all removers just bad?</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hl3560/are_all_removers_just_bad/</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1hl2fm1</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>Christmas Nails!</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hl2fm1</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1hl20hf</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>Tips for nitrile gloves?</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4nhbowgy2p8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1hl1za2</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>Rogue Laquer: Knit check??</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hl1za2/rogue_laquer_knit_check/</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1hl1via</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What's the best cheap polish you've used? </t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hl1via/whats_the_best_cheap_polish_youve_used/</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1hl1svt</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>Tips for busy person nail maintenance?</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hl1svt/tips_for_busy_person_nail_maintenance/</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1hl1b1n</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>{PR} My holiday mani with Sassy Sauce</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hl1b1n</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1hl15oj</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>Christmas nails🎄🍷</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/re9gclwxuo8e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1hl127j</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>Green for Christmas? Groundbreaking.</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kt7cgao1uo8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1hl11a1</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Happy Hanukkah! </t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vk327lrsto8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1hl0mvt</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>Please help Me Pick</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hl0mvt</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1hl0j7w</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>How often do people comment on your nails out in the wild?</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hl0j7w</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1hkzysa</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ILNP Bitten feat. shrinkage from KBShimmer QDTC </t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hkzysa</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1hkz5jn</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>beginner questions</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hkz5jn/beginner_questions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1hkz0sk</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>Does Sassy Sauce restock fairly often?</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hkz0sk/does_sassy_sauce_restock_fairly_often/</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1hkz0hw</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>Another Christmas Mani 🎄 - ILNP Frankie and Holo Taco Naughty List</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hkz0hw</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1hkynqz</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>Catholic kitsch Xmas mani</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hkynqz</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1hkydrg</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>simple christmas nails 🎄🎁</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ep2itj6a6o8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1hky4u4</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>Team red or team green?</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hky4u4</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1hky21b</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>Serpents and a Persimmon</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hky21b</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1hkxz4n</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>any tips for not picking off nail polish?</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hkxz4n/any_tips_for_not_picking_off_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1hkxx0o</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Shout out to Bee’s Knees </t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hkxx0o</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1hkxpb8</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I found this in my vault and I’m in love </t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/he0v8w290o8e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1hkxk6d</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>Christmas Mani</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hkxk6d</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1hkxh4z</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>Santa gave me a broken nail for Christmas. Better make do 💅</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xlg2f6mhyn8e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1hkxdde</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Best gold (for nail art)?</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hkxdde/best_gold_for_nail_art/</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1hkxdby</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>Opal for Christmas</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lcjmisrkxn8e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1hkxa3o</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>My favourite Nails Inc. thermal</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hkxa3o</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1hkx52o</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>Hanukkah nails 💙🤍🥰</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hkx52o</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1hkx1vz</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>Christmas mani!</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w4wuqajxun8e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1hkwlhd</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>I’m in love</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hkwlhd</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1hkwjc9</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>Softer side of Garden of Evil</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hkwjc9</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1hkwi62</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>I know people get bored with linear holos, but I can’t resist that rainbow sparkle</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bse04be9qn8e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1hkwfsc</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>Christmas mani</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hkwfsc</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1hkw888</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>finally found my purple! 💜</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hkw888</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1hkw415</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>Recomendations for sheer polishes</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hkw415/recomendations_for_sheer_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1hkw33j</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>I love the Christmas sparkle!</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/apidt4qsmn8e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1hkvw84</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>✨ILNP Chai Latte ✨</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hkvw84</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1hkvsq3</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>Holiday DIY mani</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0bgz5qfgkn8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1hkve6o</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>Christmas reds? Something special</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hkve6o/christmas_reds_something_special/</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1hkvar1</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>Emily de Molly, you have my 🩷</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hkvar1</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1hkv75h</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>OoOooo a red packed with shimmer and✨ flakiesss✨ 🥰</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hkv75h</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1hkv5vn</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>wrong holiday… oh well!</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hkv5vn</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1hkv3r6</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail art is not my forte. Here's my attempt at Christmas lights. </t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hkv3r6</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1hkuwa3</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>... holy cow</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hkuwa3</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1hktwdg</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>Happy holidays! 🎄</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hktwdg</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1hktr2y</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>I'm Wearing Peppermint Crush, so it Must be Christmastime!</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fnxwzpje3n8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1hktgw8</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>KBShimmer - Tapped Out</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hktgw8</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1hkt32r</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>State of my nails after using Holo Taco Smoothing Base consistently</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/di3hdpmjxm8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1hksngm</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>Wrapping Paper Painting 🌲❤️</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hksngm</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1hksm8k</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>My glue on nails keep popping off and my gels keep peeling off</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hksm8k/my_glue_on_nails_keep_popping_off_and_my_gels/</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1hks728</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>Has anyone known nail accessories (like the ones pictured) to disperse magnetics?</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mkpgwv4vqm8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1hks35a</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>hi guys. 💕❄️✨</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xnabk3u2qm8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1hks2k7</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>2024 in Polish: Your Top 5</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hks2k7/2024_in_polish_your_top_5/</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1hks1r0</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t xml:space="preserve">December shimmers </t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hks1r0</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1hkrjzx</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>Cuticula BF Order?</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hkrjzx/cuticula_bf_order/</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1hkrgr3</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>Ok here's mine!</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/o6pc2lezkm8e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1hkrcos</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>A Holiday Skittle to set the mood.</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hkrcos</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1hkrbo6</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>Dupes? OPI Kimono’ver Here</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hkrbo6/dupes_opi_kimonover_here/</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1hkr096</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>My husband bought me a polish organiser!</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hgamu0u7hm8e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1hkqj9m</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>Mooncat’s Star Destroyer</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hkqj9m</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1hkqaea</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>Christmas Nails this year</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hkqaea</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1hkq6t8</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Someone asked me if I’m a nail tech and I’m crying </t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hkq6t8</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1hkq3qa</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>Back to classic red just in time for Christmas!</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hkq3qa</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1hkppbd</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>✨️🎄Retro Christmas🎄✨️</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hkppbd</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1hkp5mx</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>Christmas mani 💅🏼 cute or childish?</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hkp5mx</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1hkoybd</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Last mani of 2024! </t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hkoybd</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1hkorxz</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Blue Christmas </t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hkorxz</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1hkolko</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>Hauled mulch around and not one chip🫡</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wgewxtoiwl8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1hkoke5</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>Red Velvet for Christmas?! Yes please!! ✨🎁</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3jow4rs6wl8e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1hkof1o</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>Christmas-ish</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dcean60uul8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1hko90f</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>Polish Pick Up strategy?</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hko90f/polish_pick_up_strategy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1hko6z7</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A shifty early Christmas gift </t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hko6z7</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1hkagap</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>Does this creme color exist?!</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hkagap</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1hkndrz</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>My "Christmas nails" this year 😁</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hkndrz</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1hkmrn7</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Scum And Velvety </t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hkmrn7</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1hkmg3i</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>First time trying nail art in a long time, can you tell?</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hkmg3i</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1hklu76</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>Trying to summon some Yule spirit</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hklu76</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1hklgdi</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hklgdi/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1hkl6wa</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>Dupe request</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hkl6wa/dupe_request/</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1hkkt7o</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Swamp sparrow and mistletoe! </t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6hbdd5snpk8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1hl7fs7</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>LAVENDER DOTTED DESIGN</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1hl7fs7/lavender_dotted_design/</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1hl5ggv</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>pierced christmas claws</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hl5ggv</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1hl3gvy</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>First attempt with cat eye 😅</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9qptzfo5hp8e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1hl1jc6</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>Christmas Set 🤶🏼</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ghbnzmlfyo8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1hkzuv6</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>They make absolutely no sense and I love them</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hkzuv6</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1hkxfnp</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>Hand painted Japanese Kintsugi inspired nail art</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hkxfnp</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1hkx9ik</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>Tried doing a chrome/cow print and then tried to add a pink cat eye over top ✨</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hkx9ik</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1hkwjr6</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love my nail artist. These are 3 weeks old. </t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l9mo0lpmqn8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1hkssq4</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>New nails 😍</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gv68y57nvm8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1hkv94g</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>Xmas-ish nails 💃🏻🧑🏻‍🎄</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hkv94g</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1hkv6io</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>My new nails for Christmas</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hkv6io</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1hkurr0</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>Baby boomer nails ♥️</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5ptwatktbn8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1hkt7e9</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>"preppy" lemon nails 🍋 for my 11yo niece.</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zureglixym8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1hksxr7</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>Holiday 2009 - Barbie serie season 1</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hksxr7</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1hkq7g2</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Merry Christmas! </t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pprbw8gmam8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1hkq1r0</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>just got my nails done and i’m feeling myself 🙆🏻‍♀️💅🏻</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ha4kaoxc9m8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1hkpns3</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>We’d Love Your Opinion: Quick Nail Care Survey!</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1hkpns3/wed_love_your_opinion_quick_nail_care_survey/</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1hkl7xw</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>Made a little present for my sister</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d0g7cyr6vk8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1hkl12o</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>matching nail set with my friend❤️✨</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8jffi2dmsk8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Dec 25 08:10:37 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_12_29.xlsx
+++ b/data/collected_data/2024_12_29.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C520"/>
+  <dimension ref="A1:C718"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9273,6 +9273,3372 @@
         </is>
       </c>
     </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1hlwars</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>The learning journey of doing your own gel tip nails 😭</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hlwars</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1hlw5em</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>Press ons lifting?</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hlw5em</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1hlvdjf</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Chrome silver set ✨️ </t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hlvdjf</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1hlv9vn</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>Some Cat Eye + remixed French tips by @okeinails</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hlv9vn</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1hluvrv</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>2024. What a Year✨️</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hluvrv</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1hluu70</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas nails! </t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7lyu5wnjox8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1hlutof</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>Gel, chrome, and magnetized polish Christmas holly (Rockin Around the Christmas Tree 🎶 in the background)</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2y4p6q8cox8e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1hltqc0</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>I need advice with chrome powders</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hltqc0</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1hltn5i</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>my 30th birthday is tomorrow (today for those in the eastern hemisphere) so i treated myself to my first cat eye &amp; i’m in love</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/u5tiz83g9x8e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1hltkea</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Snowy Goodness ❄️ ⛄️ </t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hltkea</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1hlt5oa</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nightmare before Christmas </t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vpzqnb7b3x8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1hlt1h9</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>🩵🤍</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ob9mu69u1x8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1hlsvag</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>Kept putting off clipping my nails and now they look too nice to cut 🥹</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/afccf1lnzw8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1hlsuy4</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My christmas nails :) </t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hlsuy4</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1hlssl3</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>new set! 😊</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jxwwz0lqyw8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1hls678</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>Industrial Grade Topcoat?</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hls678/industrial_grade_topcoat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1hls3bn</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>Speed up at home manicure?</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hls3bn/speed_up_at_home_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1hlrvxu</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>merry christmas 💅🏻</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hlrvxu</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1hlrapk</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>can i use plastic glue to reapply acrylic nails?</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hlrapk/can_i_use_plastic_glue_to_reapply_acrylic_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1hlr89j</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>Happy holidays!</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7jfoi7iufw8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1hlr0xb</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>Chrome!</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/enunpn2hdw8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1hlq0bg</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>Anyone know of a salon in Oakland, California that does this hand painted nail art on natural nails with regular polish? I would really appreciate it!💅🏻💖thank you!</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o345yd532w8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1hlplkn</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas nails </t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hlplkn</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1hlpi9b</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>Me-made Christmas nails</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hlpi9b</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1hlpfm1</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas nails </t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/e4ptg6nuvv8e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1hloixo</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Creating a 3d Christmas Snowman Set ☺️🫶🏼 Merry Christmas 🎄 </t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hloixo</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1hlndas</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>Press ons, they could never make me hate you 😍</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wnyhiem3bv8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1hlnb6f</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>Framed Christmas 🌲❄️</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xwmi6nbjav8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1hlmymq</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mani and pedi for Xmas </t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hlmymq</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1hlmwvt</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Awful Ombre </t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hlmwvt</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1hlmw9d</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>I Just Painted Them For The Holidays! 🎄</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hlmw9d</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1hllw88</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>Cute, or nah? I can't decide 🫣</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hllw88</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1hlm1za</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>Is it possible to get nails like these with normal nail polish? By @bynatashad on IG.</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x945p2fgyu8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1hlmcew</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Basic clean Christmas set 🎄 </t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s4pbnjd41v8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1hlm6o1</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>90’s French w/dark pink Beds.</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/49j791iozu8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1hlm143</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>Before and after Xmas simple gold mani to match my tree 🌲⭐️</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hlm143</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1hllnfz</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>Christmas Aqua Nails</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hllnfz</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1hlkwl1</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>christmas nails</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hlkwl1</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1hlkw3m</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t xml:space="preserve">At home manicure </t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/53x4ud9inu8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1hlkv5p</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>Best UV lamp?</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hlkv5p/best_uv_lamp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1hlk6z4</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>Just a Trans Woman Wanting to Share Her Christmas Eve Nails 🎄</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hlk6z4</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1hljnaw</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I tried the dollar tree wraps </t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hljnaw</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1hlj0ma</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>Has anyone tried the kristinacouture nails baking soda/powder/flour hacks?</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hlj0ma/has_anyone_tried_the_kristinacouture_nails_baking/</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1hlj7yg</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>Essence gel polish</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hlj7yg/essence_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1hlilhj</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>First press ons ever!!!</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vcgqpfu53u8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1hliamg</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>Christmas press ons I made❤️💚</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hliamg</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1hli6yh</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>goth christmas nails🖤🐈‍⬛</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hli6yh</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1hli3nw</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>Red nails 💅🏻</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hli3nw</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1hli1gl</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My gel nails </t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9hypciscyt8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1hli001</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Went for mermaid / ocean vibes 🌊 </t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hli001</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1hlhob4</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>Last nails of the year 🥂</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hlhob4</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1hlfq8c</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Does anyone know what’s going on with mg nail? My nail tech said it’ll grow out? </t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0jbwlafvdt8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1hle5oh</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Aussie Christmas set 🌲 </t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4kcizlubzs8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1hlc84r</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>emerald glass nails 🎄</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jfshtgsees8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1hlgdjb</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>Is lifting 1-2 weeks out normal?</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hlgdjb</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1hlhjxs</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1st time on myself, any tips?? </t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mufbucf7ut8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1hlgzfk</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>Is this a suitable shape?</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hlgzfk</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1hlhhot</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I’m obsessed 😍 </t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z3jrwuhntt8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1hlh7h8</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>Christmas nails</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hlh7h8</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1hlh3lq</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Stick-on nails </t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6brb3g77qt8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1hlh0kz</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Press on nails </t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/heksdg5gpt8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1hlgy45</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My 2024 Nail Recap✨🫶🏼 </t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hlgy45</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1hlgo9a</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>....I haven't posted in a while</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hlgo9a</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1hlgksy</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>Press ons</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x1juzmlglt8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1hlgiw4</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>Simple sparkles for the holidays</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hlgiw4</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1hlfsxd</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>Christmas nails 🥂💅</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uf9qml1met8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1hleorj</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>Feeling festive! 🎄feat. grandmas crochet stocking cat.</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nnuqnjgf4t8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1hleje4</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t xml:space="preserve">When I started going to my nail salon, there was a good bit of confusion bcuz I have the exact same name as one of their techs. She finally did my nails and absolutely knocked it out of the park bring my weird concept into reality! </t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hleje4</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1hlefeb</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I did it myself this time, what do you think? </t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/81x09pcx1t8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1hlebu3</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>my DIY holiday nails ♥️</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0lr7bcjy0t8e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1hle94z</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>Never using ASP again</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hle94z/never_using_asp_again/</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1hle20t</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Holiday set </t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nvn5gkbgys8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1hldjyg</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>My first set of press ons!!</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hldjyg</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1hldh2f</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>Christmas nails</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q2sd257kss8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1hldb7j</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time getting my nails done by a professional! What do y'all think ? </t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ujcrmlvwqs8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1hld4f0</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>Decided to try chrome this time, loveee it</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hld4f0</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1hlc3by</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>It feels like christmas</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hlc3by</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1hlbmkv</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>My new manicure - I think red is the color of passion</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1hlo6j0o6s8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1hlbf3e</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>i love french tips</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hlbf3e</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1hlarx5</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>L.A Color in Asteroid 😍</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hlarx5</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1hla2nn</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>Obsessed ❤️</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hla2nn</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1hl9epo</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>Favorite pink-ish mauve?</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hl9epo/favorite_pinkish_mauve/</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1hlwajd</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>Actually gave nail art a try for Christmas this year!</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hlwajd</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1hlw4y1</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My Christmas Day nails </t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i7dfc3m26y8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1hlvi5d</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>My toxic trait? I match my nails and my outfit (especially for special occasions)</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hlvi5d</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1hlv3dx</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I just rlly like this color </t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p0wrt92trx8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1hlv0al</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>🎶Merry Christmas, merry merry Christmas🎵</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hlv0al</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1hluovz</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Yall, help me recreate this effect! </t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hluovz/yall_help_me_recreate_this_effect/</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1hlum7r</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>My Christmas mani with gel, chrome, and magnetized polish (sound on for some Home Alone music nostalgia)</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/90nf4l1klx8e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1hltvb9</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>Sugarplum Fairy Christmas Nails!</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hltvb9</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1hltre8</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Festive Snowflake Stamp Mani </t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3plt3v5tax8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1hltmbz</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>Press on anxiety</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tnw4iak59x8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1hltlq2</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Super excited to try the thermal magnetic. </t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hltlq2</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1hlt1pz</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dupes? Or where to get this polish? It also had moon glitter and I’m obsessed. </t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s0ssi49x1x8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1hlsr2w</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>Dupe request for OPI Cosmo Not Tonight Honey</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hlsr2w</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1hlsqu4</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>Dupe request for OPI Cosmo Not Tonight Honey</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hlsqu4</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1hlsme4</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>First attempt at magnetics</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hlsme4</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1hlsdkf</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>My Christmas nails 🎄</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hlsdkf</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1hls7y2</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>How to remove stain from clothes?</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hls7y2/how_to_remove_stain_from_clothes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1hls5df</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>Christmas Pickle 🥒</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hls5df</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1hls19k</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>I need to find this color and finish</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ck250ldpw8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1hlry4n</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>Does anyone know a good grungy nail polish brand?</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hlry4n/does_anyone_know_a_good_grungy_nail_polish_brand/</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1hlr0a6</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Inspired by Dan Levi's 2024 Met Gala suit </t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hlr0a6</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1hlqw0a</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t xml:space="preserve">why is there a whisk 😭 </t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cr8q5i9vbw8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1hlqpc7</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>Merry Christmas to me from Canada!!</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gfg95cdr9w8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1hlqoz2</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Merry Christmas Eve! </t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gsrehoai9w8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1hlqa6p</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>Snagged two Helmers for $70💃</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mcouk8y35w8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1hlq2lz</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>Anyone know of a salon in Oakland, California that does this hand painted nail art on natural nails with regular polish? I would really appreciate it!💅🏻💖thank you!</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qit3d1at2w8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1hlpwjl</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>Couldn’t decide between glitter, holo, or jelly…</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mc2mcn8x0w8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1hlpw25</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>That festive feeling when your mani matches your holiday cookies 🤩🎄</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hlpw25</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1hlpu88</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>Swatch for BKL Let My Ending Be Selfless</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qkwhl5670w8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1hlp4nn</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>Holiday mani - OPI Let your love shine</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ak25830nsv8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1hlot14</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>Happy H💿l💿days!! 🎁🎄</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hlot14</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1hlo7tm</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>a very original christmas mani</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/x3g15lvejv8e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1hlo3dc</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>White, iridescent polished with a strong shift?</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d9elck47iv8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1hlnxfd</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>Flight of the monarchs 🦋</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hlnxfd</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1hlnwbt</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First set turned out better than expected! </t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hlnwbt</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1hlnrwo</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>Christmas Mani</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hlnrwo</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1hlnevv</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>Among all these beautiful Christmas manis, I decided to "transcend the trend"</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hlnevv</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1hln7o5</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>My Christmas nails!</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hln7o5</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1hlmzdu</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>Making my way through untried greens - ILNP Lucky One</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hlmzdu</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1hlmrfp</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Merry Christmas, Laqueristas! 🌲 🎅🏻 </t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rttz91275v8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1hlmqoh</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>My go-to at-home manicure this winter 😊</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0ggzioxz4v8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1hlmcm6</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Someone Convince me They’re Different </t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hlmcm6</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1hlm7j7</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>Do you use basecoat on swatch sticks?</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hlm7j7/do_you_use_basecoat_on_swatch_sticks/</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1hlm4h6</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Holiday Dark Skittle Mani </t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/39t7hbe0zu8e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1hlm1pw</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>indie brand jelly + flakies?</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hlm1pw</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1hllr0t</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>Nails keep breaking 😭</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ae9y9t6hvu8e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1hllmw0</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>Before and after subtle gold DIY mani on Christmas Eve to match my tree 🌲 ⭐️</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hllmw0</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1hllfmk</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>Christmas Eve sparkles</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/53wygrhdsu8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1hlldge</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>I really slept on this Christmas green.</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hlldge</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1hll29i</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>Happy Christmas Eve! 🎄</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ph4lzoo3pu8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1hlkz67</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Omg found a discontinued OPI polish! German-Icure! It’s ooold. </t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hlkz67</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1hlkrxl</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t xml:space="preserve">UPDATE: My husband made me a 15 day nail polish advent calendar </t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hlkrxl</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1hlkcga</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Festive green for Christmas 🎄 </t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/29d41tigiu8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1hlk8df</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>Best fake nails or thick nail polishes?</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hlk8df/best_fake_nails_or_thick_nail_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1hlk7iv</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How much Seche Restore do you typically use to thin a bottle of Seche Vite? </t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hlk7iv/how_much_seche_restore_do_you_typically_use_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1hljyqp</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>Mooncat Sin Eater is so much prettier on a full mani compared to swatched.</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hljuoz</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1hljpao</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>Mooncat Star Wars Dar Side... in need of a Light Side!!</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hljpao</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1hljice</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>Last minute festive skittle</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hljice</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1hljg8c</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>Blessed cursed pose?</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bl07korkau8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1hlj99k</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>Success away from home base! OPI Malaga Wine + Sally Hansen Unicorn top coat</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fwvmewru8u8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1hlipxn</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>Christmassy nails - might be my best yet ❄️</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hlipxn</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1hli6r8</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>Dreamscape really is dreamy</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hli6r8</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1hlhvze</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>Merry Hoho Eve!</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hlhvze</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1hlhu0c</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>Christmas shorties 🎄</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/idtbpaxkwt8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1hlhre9</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>🍬</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/221leqeyvt8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1hlhqde</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>Pastel candy canes 🍭</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jkjqb81qvt8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1hlhqa7</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>🎄</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/64yfjm1pvt8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1hlhhyx</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>I do the NYT crossword puzzle every day-- OPI gets name checked sorta frequently and I think of this sub every time!</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4cg6eypqtt8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1hlhf4v</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>Ethereal x Cracked Euphoria release</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://youtu.be/tElUBgawsbs</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1hlgbov</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>Starry night✨</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hlgbov</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1hlg2vn</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Let's talk top coat </t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hlg2vn/lets_talk_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1hlg0j1</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>Merry chrysler</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j455q0figt8e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1hlfrtb</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Merry Christmas 🎄 </t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5apnx07cet8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1hlflns</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>Gold nails for Christmas 🎄</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xtoiolbsct8e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1hlfiuw</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>Obligatory Christmas nails post</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fk0xltb3ct8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1hlfi0m</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>A Juicy Red for Christmas 🎄</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0uxfs1qvbt8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1hlfgqe</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>Snow flakies</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hlfgqe</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1hlfeg4</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>Christmas Eve nails</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hlfeg4</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1hlfarx</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>Lit</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hlfarx</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1hlevpy</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>Just another set of red holiday nails for your feeds.😆</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ooo00zya0t8e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1hleur7</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>[UPDATE] Homemade Lacquer Advent Final Reveal 👀</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9dfj34tz5t8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1hldy0b</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>the arsonist</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8b52b16bxs8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1hldg5b</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>💚 grinchy green nails 💚</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hldg5b</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1hlcx00</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>Found my 2009 nail polish stash!</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hlcx00</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1hlcpry</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Just started collecting! </t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hjf27iteks8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1hlcged</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>It's perfect😭😭 Cirque colors Lucky jelly</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wns1py3ahs8e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1hlcbu7</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>When Santa is bringing nail related Christmas presents &lt;3</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ylre18hpfs8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1hlbkz1</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Got these pretty ones for Christmas but no clue how to use them/what is needed </t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/16x9eon76s8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1hlarg6</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Merry Christmas to my polished Queens. </t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hlarg6</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1hlale3</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First try with magnetic polish! </t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x752kdo7tr8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1hl9k5p</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>it's tiiiiiime 💅🎄</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d287zslbfr8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1hks6bi</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>Christmas Finery</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hks6bi</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1hl9ivm</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>first time trying a skittle!</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/en8luukser8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1hl76r6</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first go at magnetics - a silvery festive mani </t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qeoimeuwkq8e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1hl9fzj</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Does anybody have these two shades from Sassy Sauce? I'm trying to decide if they're different enough to buy both. Dissimulation on the left, Shaken not Stirred on the right. </t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hl9fzj</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1hlv012</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>Custom Christmas Nails</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hlv012</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1hlsimf</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mix metals junk nails </t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hlsimf</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1hls9m0</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>Star of Bethlehem :)</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j041xtk8sw8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1hlqv2a</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>Christmas Snowflake Nails!</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gdum6aekbw8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1hlp7zc</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t xml:space="preserve">dreaming of a white christmas 🎄 </t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x9diu35ltv8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1hlonot</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Matching Mani Pedi! </t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hxlb910snv8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1hloj6d</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Creating a 3d Christmas Snowman Set ☺️🫶🏼 Merry Christmas 🎄 </t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hloj6d</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1hlo5k1</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>2000s style nail art</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/68ags0hsiv8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1hllco9</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>🥹🥹</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4he5nyypru8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1hlkm3s</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>Green butterfly inspired set</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hlkm3s</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1hljodd</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I tried the dollar tree wraps </t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hljodd</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1hlicos</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>Christmas press ons I made❤️💚</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hlicos</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1hlhk88</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Went for mermaid / ocean vibes 🌊 </t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hlhk88</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1hlgj75</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>Hope you all have a delightful holiday season!</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hlgj75</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1hlew1f</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>A little holiday set 🖤</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xv6e2hdc6t8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1hlduav</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>"preppy" clean girl nails 🎨 kids nowadays are crazy cause why did my 11yo niece want these "clean sade girl mature" nails.</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/myiwg0raws8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1hlddtn</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>How would you make your own press on nails?</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1hlddtn/how_would_you_make_your_own_press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1hld791</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>happy goth christmas🖤🐈‍⬛</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hld791</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1hlc2kk</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>It feels like christmas</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hlc2kk</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1hlaot4</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Snowflake Press on Nails </t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hlaot4</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1hl9mtu</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>ZEBRA PRINT DESIGN</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d586nbu9gr8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Dec 26 08:10:46 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_12_29.xlsx
+++ b/data/collected_data/2024_12_29.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C718"/>
+  <dimension ref="A1:C852"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12639,6 +12639,2284 @@
         </is>
       </c>
     </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1hmjnth</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>My fiancé likes themed nails but am running out of ideas. Here’s some from this year. Any suggestions?</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hmjnth</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1hmit0y</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>Summer growth</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o2dcswp7259e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1hmhzmv</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>I was the guinea pig for my nieces nail polish on Christmas eve... how do I reverse this?</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://imgur.com/KibVih1</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1hmh9nw</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>Christmas set</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3r88fpwzj49e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1hmgvv3</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help! </t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sn2dx6hof49e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1hmgzrg</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Glow-in-the-Dark Winter Holiday Nail Art! </t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qagpehxwg49e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1hmfzs6</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>How do they look better? Long or short?</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hmfzs6</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1hmfyvq</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Last set of the year </t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0ftvlnfl549e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1hmfj2z</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>Does this shape look professional?</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hmfj2z</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1hmffag</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>🩶❄️dark winter❄️🩶</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hmffag</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1hmfcsz</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail salons in Harrisburg </t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hmfcsz/nail_salons_in_harrisburg/</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1hmfbsb</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>Lil’ gold✨</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4fuujd3ry39e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1hmf9nw</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>First time festive nails!♥️</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0tr18xv3y39e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1hmezzn</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>NYE Nails</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hmezzn/nye_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1hmepvg</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>🐟</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hmepvg</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1hmep9j</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Chrome recommendations. </t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ugnqsko3s39e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1hmen75</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>My boyfriend's mom got me these nail art pens for Christmas, can't find the ingredients anywhere (even on the Amazon listing)</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0bs7pwyhr39e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1hmeay4</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>Christmas present from my dad 💝</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hmeay4</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1hme9mq</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>I got this nail care kit for Christmas, what do have of these do?</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qdqeafsmn39e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1hmc4z0</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Natural Nails after DIY Gel X </t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2x488hza239e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1hmdkei</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas nailsss! &lt;3 </t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hmdkei</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1hmd2yj</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>I think I like glittery nails, will have to do a few more just to make sure (a few fav sets of this year)</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hmd2yj</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1hmcyvk</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>Basic pink dip💅</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hmcyvk</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1hmbg03</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>Hyponychium Treatments?</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hmbg03/hyponychium_treatments/</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1hmch4d</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>Simple pink at home 🌸</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hmch4d</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1hmbxi8</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>UK BIAB LAMP QUERY</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hmbxi8/uk_biab_lamp_query/</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1hmbnkd</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>Christmas!!</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/psp5pkwhx29e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1hmbler</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>Velvet Magnet Roses</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hmbler</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1hmbhkr</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>Some fun gems for NYE✨</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/js279wytv29e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1hm9oi7</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Birthday nails! Merry Christmas 🎁🎄 </t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n4mw7wc1e29e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1hm9nxl</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>A Christmas Green Mani Feat. A Not Green Christmas Tree</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zpckc08wd29e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1hm9k6i</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>NYC recs to remove gel extensions</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hm9k6i/nyc_recs_to_remove_gel_extensions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1hm9hfs</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>Why did my gel X nail change colors?</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hm9hfs</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1hm8nia</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Milky white 😍❄️ </t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uuncwjm9429e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1hm7yr2</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time doing nail art! </t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hm7yr2</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1hm7ne7</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel Chipping after 4 days? </t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8jjdvwvou19e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1hm639e</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>Nails dry and peeling under gel x, is it an allergic reaction?</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hm639e</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1hm6wj2</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas set </t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hm6wj2</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1hm6pfn</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>Can I Pull Off A Holiday Set in 45 Minutes?!</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hm6pfn/can_i_pull_off_a_holiday_set_in_45_minutes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1hm6i2v</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>Merry Christmas! 🎄🎅🏻</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hm6i2v</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1hm68le</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>icy press on set🩵❄️⛄️</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hm68le</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1hm5lg9</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>Simple Christmas nails this year 🎄</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0rtuagidb19e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1hm5e3q</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>Winter nails ❄️</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j3jp5agk919e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1hm582x</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>Christmas nails matching my Christmas perfume</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hm582x</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1hm4uqn</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>Snowy mint</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hm4uqn</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1hm49ob</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>Ingredients?</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/33kfzes3z09e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1hm3u4s</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>Is this normal?</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vo9qhtp0v09e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1hm2oei</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>Cleaning press-ons?</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hm2oei/cleaning_pressons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1hm2ldq</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>owowow</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hm2ldq/owowow/</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1hm2jxk</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>Christmas Set 🎄</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hm2jxk</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1hm2fmq</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>Christmas Day nails</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hm2fmq</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1hlz01t</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help please! Nail allergy advice needed :) </t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hlz01t</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1hlz1r3</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Russian Manicure Transformation on natural nails </t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hlz1r3</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1hm23lo</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas nail stickers </t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/13k2w4hmd09e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1hm22zi</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>Dark red Christmas nails!</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hm22zi</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1hm1yis</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>Biab</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hm1yis</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1hm1s5y</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>Nails broke before Xmas so here are some short ones</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hm1s5y</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1hm1pll</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Icicle Nails ❄️ </t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/nvk6rkcc909e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1hm18vu</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>2024 nail recap 🫧♥️</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hm18vu</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1hm1119</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>A NSFW Christmas Finale</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xu41l4zl109e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1hlzqhg</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>Simple red for Christmas</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/elrszd4jlz8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1hlygw3</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Suggest tips for better rubber gel application </t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hlygw3</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1hlxan2</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Charms, molds, and stickers </t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ihpx18itmy8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1hmj9ub</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>Christmas day mani</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hmgtrm</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1hmi8g9</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>Blasphemy?</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hmi8g9</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1hmhizq</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I Choose the Bear - Bees Knees Dupe? </t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hmhizq/i_choose_the_bear_bees_knees_dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1hmgyv5</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Rave for ILNP Customer Service </t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s61lnv3ng49e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1hmfzyn</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t xml:space="preserve">i knew immediately what to use the nosferatu bucket for </t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kmyxpw8x549e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1hmfjp8</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>Christmas Haul!</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1kr2lru0149e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1hmf8yt</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>Christmas skittle 🎄</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bmyod3fwx39e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1hmeq20</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>Grinchy Flakie</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hmeq20</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1hmenll</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Compilation of my Christmas nails </t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hmenll</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1hmeh71</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>X-Mas nails from last week ft. My greasy camera🙈</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hmeh71</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1hmedp6</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>Looking for swatches of Cirque 'Kinetic' in velvet style or similar shades (magnetic burgundy) 🙏🏻</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zs2rw32po39e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1hme5nl</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What nail shape would be best for my nails? </t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hme5nl</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1hmdbrs</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>Comparing brown magnetic/metallics</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hmdbrs</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1hmczs8</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>Been waiting to wear this one ✨✨</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hmczs8</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1hmcy8a</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>This bottle of "Sealed With A Hiss" is so realistic!</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hmcy8a</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1hmcb9y</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I got tired of my Christmas manis so I tried something new with purples and golds 😍 </t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hmcb9y</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1hmc87e</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>Mooncat #2: The Arsonist</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hmc87e</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1hmc3y4</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>Anyone have peeling with Londontown Gel Genius base?</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hmc3y4/anyone_have_peeling_with_londontown_gel_genius/</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1hmbq9i</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>A Quick Xmas Mani</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hmbq9i</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1hmayhx</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>A Christmas Green Mani Feat. A Not Green Christmas Tree</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hmayhx</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1hmas8j</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>ILNP Merlot &amp; Forest Drive</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wlyj401yo29e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1hmal2x</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t xml:space="preserve">One of the most beautiful polishes I own </t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hmal2x</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1hm974i</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>Hit the jackpot this Christmas!</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hm974i</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1hm8ygj</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>Recommendations for blue and white nail polish for porcelain nails?</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0jv5kub0729e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1hm8s57</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>Christmas Cheer Nails ft. Dam Nail Polish 💅</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bc1nurgf529e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1hm8bod</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails for the week, it’s a nude Xmas for me </t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hm8bod</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1hm7xjj</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>🎄Last Min Christmas Mani🎄</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hm7xjj</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1hm7wx0</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>Mega (X) looks like TV static 🥰</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hm7wx0</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1hm6za7</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Got this present today! 😂 🕎</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/677zmbwbo19e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1hm6msx</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas Mani </t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hm6msx</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1hm6j24</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t xml:space="preserve">hardcore, right? 😂 </t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v2j610a8k19e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1hm6fya</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>November/December nails</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hm6fya</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1hm5z7v</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>Festive metallic mani 🎄</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hm5z7v</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1hm58vc</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Merry Christmas 🎄 </t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hm58vc</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1hm4wey</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>(PR) First night of Hanukkah nails! 💙✡️</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hm4wey</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1hm48pm</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>Christmas tinsel, or metallic pesto?</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hm48pm</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1hm3xkp</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas nails. </t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/su6tcvsxv09e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1hm3te0</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Accidentally matched these earrings kind of </t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hm3te0</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1hm3ld5</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>Merry Chrysler!</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hm3ld5</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1hm3fmu</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>🎶 i’m dreaming of a pink christmas 🎶</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hm3fmu</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1hm30gi</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>Glazed chocolate donut nails with regular polish</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qvc3in2wm09e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1hm2nj4</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>Happy Holidays, everyone!</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hm2nj4</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1hm2103</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>Received the Manicurist Actives set for Christmas 🎄💅</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hm2103</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1hm1s64</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>🎄Gingerbread🎄</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hm1s64</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1hm1rps</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>Christmas/birthday mani</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hm1rps</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1hm1kek</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>Happy Holidays from Candy Cane Lane</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hm1kek</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1hm170s</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>Northern Lights</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ua2uvetj309e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1hlzp58</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>777’s time to shine ✨</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/kk9l8zs0lz8e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1hlznll</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>Mooncat forbidden fruit</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hlznll</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1hlz939</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Jingle Dress Dreams 👗 </t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hlz939</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1hlc9ru</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>UK based beginner</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tgj1f5bzes8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1hlfns4</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>nails at home with cats</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hlfns4/nails_at_home_with_cats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1hlj7hp</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>Loving MAGNETICS!!!</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2ncyrpge8u8e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1hlm2eb</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>Soft gel press ons + HEMA</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hlm2eb/soft_gel_press_ons_hema/</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1hloc38</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>🎀🌸🩷 Yule nails ☀️🌲🍊</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hloc38</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1hlpxiu</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Holiday nails </t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hlpxiu</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1hlyv6q</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>Flakie 🎄, happy holidays to you all 💖</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hlyv6q</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1hly99h</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>Merry Christmas!</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hly99h</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1hlwspd</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Thank you for helping me have healthy, long-ish, beautiful, natural nails for my engagement! </t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xy8h0nmgfy8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1hmj51a</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>Try out one of my favourite press on nails</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hmj51a</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1hmi5c7</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t xml:space="preserve">my new set :3 </t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hmi5c7</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1hmgygu</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>Jinx arcane inspired nails</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/abs3mdbig49e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1hmeq60</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>Product help!</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1hmeq60/product_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1hmabjt</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>Merry Christmas and Happy Harlidays!!❤️🖤💚</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hmabjt</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1hm9ge3</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>Here nail for baby shower! 💙</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/meld9ryvb29e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1hm7ocw</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My new Christmas nails! </t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hm7ocw</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1hm5n2f</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Merry Christmas AND happy new year set </t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hm5n2f</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1hm518b</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>Can I Pull Off A Holiday Set in 45 Minutes?!</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1hm518b/can_i_pull_off_a_holiday_set_in_45_minutes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1hm3sq1</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>I love my manicure, it looks like jelly, what do you think?</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ukap6cwlu09e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1hm1ww1</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>Christmas Set</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hm1ww1</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1hm0t08</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>Christmas Nail Art</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ai7fhv0zz8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Dec 27 08:10:32 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_12_29.xlsx
+++ b/data/collected_data/2024_12_29.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C852"/>
+  <dimension ref="A1:C1015"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14917,6 +14917,2777 @@
         </is>
       </c>
     </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1hn9l6i</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>Beautiful pink hand nails to match my toenails</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j96dg2v2ec9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1hn8ui6</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Newbie with a dumb question </t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hn8ui6/newbie_with_a_dumb_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1hn8jbw</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>Best thick, full coverage glitter nail polishes?</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hn8jbw</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1hn7zak</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>90's Nail Tips</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hn7zak/90s_nail_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1hn802u</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>Absolutely loved this set! 🍋‍🟩</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hzg5m7gjvb9e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1hn7kfu</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel x tips </t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hn7kfu/gel_x_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1hn7hmz</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>AriZona press-ons from Kiss Nails</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0gn3cd93qb9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1hn6xav</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>cuticle care help</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hn6xav</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1hn6hf3</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Recommendations for quick drying, thick, easy nail polish? </t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hn6hf3/recommendations_for_quick_drying_thick_easy_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1hn5i87</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>Why does my nail grow like this?? Help!!!</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hn5i87</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1hn4xnc</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>my christmas nails are gone! (sad) now it’s time for wintery ones! ❄️</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ndr19sdj0b9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1hn6082</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t xml:space="preserve">White marks on nails </t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hpstav6zab9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1hn5kmg</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>XMAS set w/ Boyfriend :)</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/41q2hryo6b9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1hn4x0i</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>My Christmas Nails</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cgyduhcc0b9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1hn4qrk</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>Press On/Acrylic Help</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hn4qrk/press_onacrylic_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1hn4kpw</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>My natural nails have finally come back somewhat healthy!</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/513igvx2xa9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1hn497w</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>You guys were really awesome about my scene nails last time, so here are the nails I did for Christmas!</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hn497w</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1hn3iwp</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>D.I.Y Press Ons</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hn3iwp/diy_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1hn30ml</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>Did my moms nails before christmas</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bh3ghnukia9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1hn2vmf</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>Champagne pop nails for New Year’s ✨</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hn2vmf</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1hn2u10</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>Nails to bring in the new year 🎉</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pv5wsokyga9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1hn2qlt</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Do you like these? </t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/opvkpo16ga9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1hn2k48</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Years of my Christmas Nails </t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hn2k48</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1hn2clq</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>Gel X chipping</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pjxmr07sca9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1hn0rg0</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Amateur at home rubber base gel, worried about potential allergy </t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hn0rg0/amateur_at_home_rubber_base_gel_worried_about/</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1hn0t7h</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Recommendations </t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hn0t7h/recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1hn1kk8</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>What the best way to avoid contact dermatitis?</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hn1kk8/what_the_best_way_to_avoid_contact_dermatitis/</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1hn150j</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>first time acrylics too thick? professionally done</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hn150j</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1hn0nhn</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>what shape of nail extensions suit my hands the best?</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hn0nhn</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1hn0mh4</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>Strawberry Jelly 🍓</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hn0mh4</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1hn0oec</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>Christmas Nails 🎄</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w43xdzkdy99e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1hn0c8d</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Russian milky white manicure 💅 </t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dgjx198mv99e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1hmzu4v</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Opal but a nail </t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hmzu4v</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1hmzf3i</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail dryer machines </t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hmzf3i/nail_dryer_machines/</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1hmz69c</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t xml:space="preserve">UV press ons help </t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/atubwgewl99e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1hmz6ix</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t xml:space="preserve">DIY Help </t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hmz6ix/diy_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1hmz6bi</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>2024 nails</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hmz6bi</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1hmz3tb</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>Which colour would suit my nails the best?</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uksf0n0cl99e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1hmz2jm</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>Thin nail solutions?</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hmz2jm/thin_nail_solutions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1hmyvto</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>First polish manicure in years</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5u2187nij99e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1hmylu7</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>Are nail salons always really smelly or am I just sensitive?</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hmylu7/are_nail_salons_always_really_smelly_or_am_i_just/</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1hmxp9u</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>Snoopy nails</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hmxp9u</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1hmxotx</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>Tbf I do my own nails</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hmxotx</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1hmxiqz</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Baby blue chrome </t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hmxiqz</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1hmxcei</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New Year's eve nails done by my little sister. I'm so happy with them. </t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/trbek5f6799e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1hmx8z6</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>beginner: how can i improve?</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nj2eiyle699e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1hmwp3w</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>Sally Hansen Insta-Dri technique</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hmwp3w/sally_hansen_instadri_technique/</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1hmwzaf</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>Happy Holidays! Here are my Christmas Nails</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hmwzaf</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1hmwvnh</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>winter vibes over here ❄️☃️🩷</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e3dfk0xc399e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1hmwttp</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>Wedding ready!</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2uzuoi4y299e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1hmwsjw</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>Magnetic polish- minus the magnet 😂</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/blenzajm299e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1hmvk9g</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>Please help me find the right red!</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hmvk9g/please_help_me_find_the_right_red/</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1hmvlqn</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tacky Christmas nails </t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hmvlqn</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1hmvzdb</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>My Christmas nails! 🎄😁</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4xqqom76w89e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1hmvwtn</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Went with short ballerinas for new year </t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hmvwtn</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1hmvu6u</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>gel x done at salon popped off 3x in 5 days. my fault??</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hmvu6u</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1hmvc0y</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>My nails for 2024</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hmvc0y</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1hmv9kj</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>finally painted after years- and why i don’t paint them more.</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hmv9kj</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1hmv919</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>Which grit is used for nail prep, and which grit is used to file acrylics?</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hmv919/which_grit_is_used_for_nail_prep_and_which_grit/</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1hmv5sb</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ex biter </t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xsq0yu8mp89e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1hmur73</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>Gel X Cateye</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r6gt6zqcm89e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1hmuozd</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>beginner 🫶🏼</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l8jgjvztl89e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1hmu7lh</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>Gel won’t stay on</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hmu7lh/gel_wont_stay_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1hmtnqu</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Queen of Heart Nails </t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ag9fm7sjd89e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1hmtlc7</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>nails for 17th birthday</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/kx7sbt10d89e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1hmo1u1</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>HELP NEEDED: CLIENT REQUESTING REFUND</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hmo1u1</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1hmnigu</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Press on alternatives. </t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hmnigu/press_on_alternatives/</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1hmtggc</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Recommendations? </t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tt17zeqvb89e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1hmt1sh</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>Christmas 💅 💙🎄</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hmt1sh</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1hmrty6</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>Snowy Night Nails ❄️🌙</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hmrty6</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1hmrsvi</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>Nude, only nude</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b3x67gqjy79e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1hmrs99</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>Oh my god 😍</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8v3hzfdey79e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1hmro4d</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>Im scared of going to a nail salon</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hmro4d/im_scared_of_going_to_a_nail_salon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1hmrkxi</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>strengthening nails. my works for December</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dncus5pqw79e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1hmqr1b</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hard gel nails. </t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/81u6omztp79e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1hmprpv</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>Painted my nails (shaky hands were bc of Monster Energy)</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/088opc27h79e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1hmpbyo</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>Holiday nails // How to make sure these decals stick?</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://i.imgur.com/r7TJX76.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1hmovav</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I spent way too long making my Christmas nails 😮‍💨 </t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hmovav</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1hmogiz</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>squishmallows are my fav so ofc I had to turn them into nails 🎄⛄️</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hmogiz</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1hmoejs</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>Finally got around to making my own christmas nails 🍪🎀</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hmoejs</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1hmnl1b</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>Birthday set</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7y1dzgbou69e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1hmmt9i</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>Holiday nails</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hmmt9i</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1hmmnsq</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>Acrylic Nails set for November ❤️</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pjjaujofj69e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1hmm5vj</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>First time doing Gel-X at home</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hmm5vj</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1hmlsll</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>Hi Girlies, just "Just nailed it! 💅✨ #FeelingPolished 😭❤️😆</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tgjp97sn769e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1hmlfos</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Best non damaging nail glue - Canada? </t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hmlfos/best_non_damaging_nail_glue_canada/</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1hml8d1</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t xml:space="preserve">my bf got me a gel nails kit for christmas! this is my first time ever doing my own nails, how did i do? </t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rk68ajh0069e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1hmkuy5</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>I've been getting BIAB for 18 months and my nails are suddenly breaking - bad luck, or do I need to take a break?</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hmkuy5/ive_been_getting_biab_for_18_months_and_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1hmkifg</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>le mini macaron set keeps peeling?</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hmkifg/le_mini_macaron_set_keeps_peeling/</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1hn7fm3</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>Fake Halo 🌈🌟</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hn7fm3</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1hn66gk</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>Winds of Fate Dupe?</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hn66gk</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1hn65rt</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>Just need to share my pain 🥲</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hn65rt/just_need_to_share_my_pain/</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1hn5ve0</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>ILNP U Magnet</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hn5ve0/ilnp_u_magnet/</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1hn5ldn</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>Nail polish always chips IMMEDIATELY</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hn5ldn/nail_polish_always_chips_immediately/</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1hn5ctb</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Looking for a navy nail polish similar to the photos below? </t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/om60u3ck4b9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1hn5b3t</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>*update* it took 4 hours but I am so happy!!</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hn5b3t</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1hn59kx</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>Cirque Colors - Chroma Rose</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hn59kx</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1hn56y8</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>Professional grade gel polish that doesn’t need a license to purchase</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hn56y8/professional_grade_gel_polish_that_doesnt_need_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1hn4ww9</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>Aquaberry by fancy gloss</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/85apo2ac0b9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1hn4l0c</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>Thank you SO much for the gel allergy advice/info</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hn4l0c/thank_you_so_much_for_the_gel_allergy_adviceinfo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1hn44ri</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>Grayscale nails for Nosferatu!</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hn44ri</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1hn3vqc</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>New to long nails and I have some potentially stupid questions</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hn3vqc/new_to_long_nails_and_i_have_some_potentially/</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1hn3uk9</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Really getting into magnetics lately </t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2yj9458bqa9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1hn3p7u</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>Stages of Ouzle by Death Valley Nails!</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hn3p7u</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1hn3ga3</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>How do I get professionally done polish off?</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hn3ga3/how_do_i_get_professionally_done_polish_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1hn334o</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>Found Essie for $1.50 a bottle on eBay💃</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hn334o</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1hn30dh</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>Good organization recommendations for a moderate sized collection? (130 polishes)</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hn30dh/good_organization_recommendations_for_a_moderate/</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1hn2unl</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>Soft glowy look after Christmas</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hn2unl</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1hn2ptw</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>Shrinkage after adding thinner to QDTC?</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hn2ptw/shrinkage_after_adding_thinner_to_qdtc/</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1hn2kf1</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>Christmas nails</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vhap4ndoea9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1hmq7mg</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Reflective polish on gel extensions 🖤 </t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hmq7mg</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1hn0s5y</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>This belongs here</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/87tsr897089e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1hn0ndo</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>Serpents of Eden is everything people say it is 🐍💚</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hn0ndo</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1hmzsck</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>Spacing out after Christmas celebrations :)</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/k8k7sumyq99e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1hmzhit</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Glimmer ✨️ </t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hmzhit</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1hmzfq2</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Organizing my Tackle Box - the perfect afternoon </t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hmzfq2</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1hmzeco</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>Help, what shape should I file my nails?</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hmzeco</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1hmyrnm</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>Nail polish wears off within a day</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hmyrnm/nail_polish_wears_off_within_a_day/</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1hmyiaa</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>I can't be the only one who feels this way</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ayc9hcmkg99e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1hmy8x8</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>Didn't have time to do a Christmas mani so here's my day after Krampus mani instead</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hmy8x8</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1hmy0qc</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>Perfect Christmas Red</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hmy0qc</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1hmy0f7</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>Super fine sheer shimmers?</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hmy0f7/super_fine_sheer_shimmers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1hmxupc</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Base coat to survive chlorine? </t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hmxupc/base_coat_to_survive_chlorine/</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1hmwkzl</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>What was used to create this look?</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hmwkzl/what_was_used_to_create_this_look/</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1hmwia1</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>My mooncat order</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4f1qnhxe099e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1hmwece</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>Whiskey Sunrise is stunning</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hmwece</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1hmw6g1</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>Happy Hanukkah 😊</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o2urchkqx89e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1hmvpl9</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>Got the new Mooncat Darth Vader Collection!</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pfnmubmzt89e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1hmvdjj</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>Baby’s first Christmas mani 🥹</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hmvdjj</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1hmv8k5</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How I’m spending my day! </t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hmv8k5</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1hmuteg</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>Emily de Molly- Perfect Score! 💜</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9uqwc5tum89e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1hmukgc</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>Naughty and Nice mani ❤️💚</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hmukgc</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1hmujkr</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>Where to find magnetic nail polish in Paris</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hmujkr/where_to_find_magnetic_nail_polish_in_paris/</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1hmtz30</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>Worst Christmas Gift ever</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hmtz30</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1hmtulw</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>scene kids are alive and well xD!!</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hmtulw</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1hmsms9</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>My first Mooncat polish!</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4903fcn7589e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1hms3si</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Please help me to get a nail polish similar to this color </t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hms3si</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1hms1c9</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>🕎Happy Hanukkah🕎</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hms1c9</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1hmrwi4</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>Which nail polish shades are going to beautify your fingertips in January? These are my choices:</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/858ggukcz79e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1hmrld2</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Shipping issues, USPS specifically </t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hmrld2/shipping_issues_usps_specifically/</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1hmquwx</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>(PR) All wrapped up for night two of Hanukkah 🎁✨🎀</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hmquwx</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1hmpz0a</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>Christmas Gold</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hmpz0a</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1hmpppq</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Do any of you ever touch up just your free edge on your manicure? </t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hmpppq/do_any_of_you_ever_touch_up_just_your_free_edge/</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1hm1b8h</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>Hardest Part of Growing Nails</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hm1b8h</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1hmnpz2</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Am I right to be upset with how a tech removed my gel extensions? </t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hmnpz2/am_i_right_to_be_upset_with_how_a_tech_removed_my/</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1hmnoe6</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>Manicures - How Long Do They Take?</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hmnoe6/manicures_how_long_do_they_take/</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1hmlw44</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>My Rogue mystery holiday nail haul ft. kitty helper</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hmlw44</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1hn5zgh</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>Recommendations for nail tools and brands</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o2v5gthrab9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1hn8nvv</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>My first Soft gel nails</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/48js2jjt2c9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1hn8czx</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>Hand drawing is difficult ... but cute!</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cd8l0m88zb9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1hn5h3k</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My younger one’s Nail extensions set-She’s still a trainee nail tech.all feedback/recommendations are welcome 🤗 </t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5u5u201q5b9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1hn5f16</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>A little sophisticated beauty in the world of French nails.</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hn5f16</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1hn2z30</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My beach nails by @eloubeauty </t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x1p3t8w7ia9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1hn1tts</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>Doing my nails for 3 months now</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hn1tts</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1hn0n9e</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Strawberry Jelly </t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hn0n9e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1hmyfde</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My Christmas nails are so cute 🎄 </t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tfdp5ddxf99e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1hmxs36</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>Help me get started with nail art!</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hmxs36</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1hmtyy7</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>Pop art nails. Is anyone else constantly changing their design because they're never satisfied?</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hmtyy7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1hmrsxg</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My Christmas nails </t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1hmrsxg/my_christmas_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1hmquba</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mermaid </t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z3e1n6llq79e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1hm341n</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>Merry Xmas</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/idkrheyxn09e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1hmmzvt</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My younger one did the set,she’s still practicing #AcrylicNails </t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qs0f22wmn69e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1hmmpev</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>My Younger sister who is still practicing did this set for me. Please leave suggestions and feedback 🍀</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ln08vq21k69e1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Dec 28 08:09:23 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_12_29.xlsx
+++ b/data/collected_data/2024_12_29.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1015"/>
+  <dimension ref="A1:C1204"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17688,6 +17688,3219 @@
         </is>
       </c>
     </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1ho0uue</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>This sub just popped up in my feed, so I thought I'd share. I'm a middle-aged man with Christmas hands. Bad hotel photographs don't do them justice.</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ho0uue</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1ho01e8</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Advice on polish choice </t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ho01e8/advice_on_polish_choice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1ho0hou</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>Before and after (nail biting)</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2cw1jt9bij9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1ho0ftx</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>Xmas nails 🎄🥰</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9qlk5dbohj9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1ho0afx</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>Bright! Bold! Brilliant!</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ho0afx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1hnzwb4</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>Nail Lift: Not near original salon</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hnzwb4/nail_lift_not_near_original_salon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1hnzs1q</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Love nails 💅 </t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3j6dmttk9j9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1hnzpxi</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did my sisters nails </t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hnzpxi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1hnzpb9</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love my Christmas dip set and I think my nail tech did a great job. I am so grateful! </t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hnzpb9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1hnz8ge</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Should I break up with my nail tech? </t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hnz8ge/should_i_break_up_with_my_nail_tech/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1hnz6xt</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>My friend is so talented 🫶🏻</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hnz6xt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1hnyyt8</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>These are BADASS</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bqk5raje0j9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1hny6o6</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>Nails Look 💅</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pxhoroq9si9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1hnxwo6</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>Need advice on finding independent nail techs!</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hnxwo6/need_advice_on_finding_independent_nail_techs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1hnx42p</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>Rose gold chrome 💕✨</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hpdxkb1ahi9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1hnws3c</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love red nails </t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gt5x4l5xdi9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1hnwon8</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>New Year’s vibe</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/clherkszci9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1hnwoai</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>Galaxy set</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hnwoai</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1hnwla3</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>Made this set for a customer!</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hnwla3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1hnuf69</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>How do you choose?</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hnuf69/how_do_you_choose/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1hnw8rz</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>Can I get acrylic removed and then just have natural short nails painted?</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hnw8rz/can_i_get_acrylic_removed_and_then_just_have/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1hnw596</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>Is this color business professional?</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jpahb1vr7i9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1hnw3u3</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>Help! My nails aren’t growing how I want</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hnw3u3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1hnvu7w</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>Fire Emblem Fates Leo as Stained Glass Painting Nail Art!</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hnvu7w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1hnvjsb</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>Wintery pretties</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hnvjsb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1hnvi06</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>first set of kiss press on nails!!</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hnvi06</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1hnvao1</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>Wedding nails trial</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/60dsr9ukzh9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1hnuqq4</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>💕💗💖💝💓</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hnuqq4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1hnuq2s</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>Rhinestone placement advice?</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ubcih389uh9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1hnudpw</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>Love how these look</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hnudpw/love_how_these_look/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1hnu0te</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>Dragon Eye Nails</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hnu0te</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1hntpok</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New nails </t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0949by70lh9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1hnt6ay</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>is jodsone gel polish safe?</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hnt6ay/is_jodsone_gel_polish_safe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1hnsu7g</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>My very first time doing my own gel x nails!!!! So excited abt how they turned out 🤭</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hnsu7g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1hnssgm</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>Looking for a baby pink gel polish like this that is not sheer!</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cbp4cxoxch9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1hnsaum</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>I was going for a classic vintage red almond ❤️🖤</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hnsaum</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1hnrr9w</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t xml:space="preserve">UV lamp exposure and “breaking up” with my nail tech? </t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hnrr9w/uv_lamp_exposure_and_breaking_up_with_my_nail_tech/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1hnrnya</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>Didn’t like the chrome trend at first but 😍😍😍</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hnrnya</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1hnrdre</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What shape would look best on me? I have smaller, stubbier hands. </t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hnrdre</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1hnr0mj</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>First time glue-ons</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hnr0mj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1hnqqbs</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time using gel polish! </t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x0irbgwsvg9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1hnq90w</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Thoughts on these NYE nails! </t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r503v1m0sg9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1hnq2ae</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Builder Gel with Regular nail polish - What am I doing wrong? </t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hnq2ae/builder_gel_with_regular_nail_polish_what_am_i/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1hnpyn7</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t xml:space="preserve">another simple acrylic set I did myself ! </t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a0bijvfopg9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1hnpgip</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>some of my nail sets from the past✨✨</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hnpgip</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1hnok7a</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>Help! Can someone recommend a regular non gel polish that will give me the lavender milk look??</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zid1hjuleg9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1hnoxku</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>what do we think?</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uymy21tihg9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1hnos0e</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>My former nail artist always said all glitter is too much for a grown up. But this time I went all out and got what I wanted. Please tell me what you think?</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hnos0e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1hnovjs</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>Xmas nails ♡</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hnovjs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1hnorfu</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>Best kit for no polish natural nails?</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hnorfu/best_kit_for_no_polish_natural_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1hnoodh</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>Wedding nails trial</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hnoodh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1hnogdj</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>Any tips on my nails</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hnogdj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1hno68c</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>Blue 💙💙💙</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hno68c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1hno5iq</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>Blue 💙💙💙</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hno5iq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1hnnrln</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Non traditional </t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lrprbf198g9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1hnnb1v</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>Square or almond</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hnnb1v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1hnnamr</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>Bruising and allergy to doing Beetles gel at home.. Anyone else experiencing this? What are my options for nails going forward?</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/exnihgki4g9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1hnn251</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail tips or forms? </t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hnn251/nail_tips_or_forms/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1hnmjiw</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love a little sheer in my nails </t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f4wcxgejyf9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1hnm2m7</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>Why is my gel x goopy?</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5vwh807xuf9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1hnmf11</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A design that I made in Hallowen </t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hto8ndxjxf9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1hnmdq7</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>OPI Machu Peach-U</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hnmdq7/opi_machu_peachu/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1hnix4k</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>Why does my nail grow flat on one side and then curve sharply down?</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hnix4k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1hnl6w5</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>Help finding inspiration</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hnl6w5/help_finding_inspiration/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1hnlflt</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>First time getting a manicure.. coworker wrote my instructions. Good for engagement shoot?</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hnlflt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1hnl25d</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>My natural nails, thanks to Gel X!!</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/26uance3nf9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1hnl0l8</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>What shape would be best?</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hnl0l8/what_shape_would_be_best/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1hnk5uv</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>How to ask for builder gel?</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7xkej856gf9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1hnjp6p</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>Red and black set</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hnjp6p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1hnjemw</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>🌙✨⭐️ Nails</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hnjemw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1hnitbd</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>first time getting my nails done</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hnitbd/first_time_getting_my_nails_done/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1hnes49</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>Tried Beetles Gel Polish - Disaster</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hnes49/tried_beetles_gel_polish_disaster/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1hnf8km</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>Update to: Is this normal? Paid €45 for crappy nails</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hnf8km</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1hngp46</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>Help needed, are this signs of primary onycholysis?</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hngp46</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1hni3cx</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>Silver New Year nails, 35€ *_*</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/oy1izz120f9e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1hnhl8h</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>New nails 🤍✨</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/346cyaezve9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1hngv4v</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>My birthday is coming up so I did my nails! What do we think?</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wnkvibx1qe9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1hng8h6</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>Purple appreciation 💜</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hng8h6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1hnfbca</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>Blooming gel &gt;&gt;&gt;&gt;&gt;&gt;&gt;</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jqhem02bce9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1hnf7xc</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>First acrylic nails - now what</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hnf7xc/first_acrylic_nails_now_what/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1hnf52o</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>Hello everybody! I just wanted to share with you my festive nails</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y5gzde7mae9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1hnf44z</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>Asked my sister to do something festive to my nails for the New Year ✨</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wiccc8gdae9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1hner48</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>ISO short tips for my wide .60inch /15mm thumbs</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hner48/iso_short_tips_for_my_wide_60inch_15mm_thumbs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1hndl76</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>First chrome set 🥰</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7z4j3f29ud9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1hndgei</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>new vs. 3-week old press-ons</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hndgei</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1hnc56o</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>Winter nails !! ❄️</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zkebwye2cd9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1hnzxez</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>Oil Soak Wisdom Needed 🙏🏻</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hnzxez/oil_soak_wisdom_needed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1hnzuvk</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>Can quick drying top coats like Essie “Good To Go” cause chipping?</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hnzuvk/can_quick_drying_top_coats_like_essie_good_to_go/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1hnznoh</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>Which magnets are your favorites to use for magnetic polishes?</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hnznoh/which_magnets_are_your_favorites_to_use_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1hnzaj1</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>Please recommend a few ILNP polishes that can work as sheer topcoats over creme polishes I already own</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qmb7txy04j9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1hnz6o2</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>My first magnetic that’s not just a swatch!</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/oyi5bmeu2j9e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1hnys89</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>Pink Void Nails 🩷🖤</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1a3azs7fyi9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1hnyls7</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>Xmas Mani</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hnyls7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1hnxhic</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>still got on my Christmas nails, anyone else?</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3xtw5muyki9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1hnxha1</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>Magnetic setup + ILNP Deep Space</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hnxha1/magnetic_setup_ilnp_deep_space/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1hnwypa</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>OPIxWicked Nessa-ist Rose &amp; Love You So Munchkin</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hnwypa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1hnwxp8</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Favorite top/base coats? </t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hnwxp8/favorite_topbase_coats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1hnwhik</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>Christmas gift hype</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bf4zjzz0bi9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1hnwgum</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>OPIxWicked Oh, For Oz Sake</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hnwgum</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1hnw6mw</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>Too bad I don’t have enough gems or patience to do all my nails like this (tourmaline,aquamarine,amethyst and citrine)</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hnw62j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1hnw4cp</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ephemera - Alchemy Lacquers </t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hnw4cp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1hnvzlx</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>Anyone else disappointed in the Cracked and Ethereal collab?</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hnvzlx/anyone_else_disappointed_in_the_cracked_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1hnvn9p</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>Merry Belated Christmas!!</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/75uzld6u2i9e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1hnvjd6</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>Never realized shimmer polishes were made in the 1930s!</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://youtube.com/shorts/8nMTLiWqpdM?si=38o1riVpCbZhOhUI</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1hnvi75</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>manicure newbie questions pls be nice</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hnvi75/manicure_newbie_questions_pls_be_nice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1hnvfcz</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>easy nye design ✨️🖤 *contains some gifted pr*</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hnvfcz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1hnveys</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>One Brown</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hnveys/one_brown/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1hnvajl</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fresh Manicure </t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hnvajl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1hnv65s</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>My nails have a long free edge for a fleeting moment so I had to use one of my fave thermals</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ixvcyq6eyh9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1hnuthx</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>Do I have contact dermatitis?</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hnuthx/do_i_have_contact_dermatitis/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1hnuird</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>Looking for a dark bronze</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hnuird/looking_for_a_dark_bronze/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1hntu7j</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>❄️ Swatching the Winter Fantasy Collection by Glam Polish [gifted PR]</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://youtu.be/77BJMlqN43s?feature=shared</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1hnt43a</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Polish thinner for peel off base? </t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hnt43a/polish_thinner_for_peel_off_base/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1hnt39w</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>Swatched my collection</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hnt39w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1hnszxr</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>Okay Sabertooth 😍</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xbhcn18t289e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1hnsqpt</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Onism </t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lt1wtynkch9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1hnsk2p</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>One year...</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hnsk2p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1hns99l</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>Looking for a gel polish that is this color pink and is NOT sheer. Pls help I’ve tried so many!</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w3llague8h9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1hns5lx</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>The mummer’s dance</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hns5lx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1hnrx29</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>Love at first sight</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hnrx29</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1hnrvq8</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>Alchemy Lacquer BF haul</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hnrvq8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1hnrpo7</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>Tree Sentinel</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/exkqh7xr3h9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1hnrm9t</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>Lovingly named my Elsa Nails</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hnrm9t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1hnrfui</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>Mooncat bottle broke 🥺</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qzwhdz6k1h9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1hnrft6</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Does anyone have swatches of Lurid Lacquer’s the joy of snow? </t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hnrft6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1hnre7w</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>Dance of the Sugar Plum Fairy</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hnre7w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1hnrc9h</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gnome for the holidays </t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jtnw4luq0h9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1hnr67b</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>This is an old Hard Candy nail polish from the 90’s but I love it</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hnr67b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1hnr5n9</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>Got my PPU order!</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hnr5n9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1hnr42q</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>New Year's Blue</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7jmgpzawyg9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1hnr0c0</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>Jinxed! 🔮💜✨🌙</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hnr0c0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1hnqy25</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mooncat Star Wars: out of this world! </t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/l2o0aiyixg9e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1hnqtjh</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>Darkened Trail felt appropriately blue today</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hnqtjh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1hnojhx</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>✨️💚Wrapping Paper💚✨️</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hnojhx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1hnofub</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I just love Bees Knees </t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hnofub</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1hnoeed</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>Broken</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sg0rr1nbdg9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1hnobsi</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>Checking a few days late with my Christmas mani</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hnobsi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1hnob71</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>Glitter and gloss topcoat advice</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hnob71/glitter_and_gloss_topcoat_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1hnnu45</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t xml:space="preserve">[Mini rant] I'm tired of how the most gorgeous Ethereal polishes are always mysteries. </t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hnnu45/mini_rant_im_tired_of_how_the_most_gorgeous/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1hnn37z</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Holiday Nails </t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hnn37z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1hnmlv5</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>December Wrapped</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hnmlv5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1hnll4m</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>Last night acetone dissolved the cheap eyeshadow brush I used for clean up. Any recommendations for a good brush?</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rjb56uq3rf9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1hnl7e2</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>Pure Joy giving me pure joy</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hnl7e2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1hnl07o</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>First cateye ft. Blade of the Frontiers</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hnl07o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1hnkvdm</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>Me not checking how much I've actually spent on polish so that the number is forever 0</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ix07y0rbze9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1hnki0m</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t xml:space="preserve">star wars collab!! </t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/c46n846tif9e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1hnk5m6</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>Wicked Nails</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/09zmkty3gf9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1hnjsm4</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A surprise in my stocking </t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qoz0lcuadf9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1hnjm1s</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>Brand recommendation for micro flakies and shifty shimmers</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hnjm1s/brand_recommendation_for_micro_flakies_and_shifty/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1hnjk4g</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>How the heck do you swap out the brushes on Zoya bottles?!?!? 😵‍💫</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hnjk4g/how_the_heck_do_you_swap_out_the_brushes_on_zoya/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1hnjbaa</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>What are your least favorite finishes/components?</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hnjbaa/what_are_your_least_favorite_finishescomponents/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1hnj7ie</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>Nail polish off of Etsy?</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hnj7ie/nail_polish_off_of_etsy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1hnijxq</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>catrice - stargazing</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0heho60p3f9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1hniib2</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Flower Child - Worth The Hype + Orly Bonder Rant </t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hniib2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1hnihi4</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>Broken nail!middle finger 😭 Redrum, Shleee polish. Lovely Christmas present!</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jh8nhni63f9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1hnigl0</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>Proof of the afterlife</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/857vh8az2f9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1hnhk11</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>(PR) Rugelach-inspired nails for Hanukkah 🥐🤎</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kng3q3vpve9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1hnh62f</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>How does this shape look? First time trying anything other than square/squoval.</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gaj73owmse9e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1hnh3f2</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>Here’s one for everyone on a no-buy</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6jr0nd00se9e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1hngvbb</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>ILNP Deep Space: Consider me INFLUENCED 😍</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8q4cz7q3qe9e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1hngdcp</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>ILNP Neon Rosebud base color showdown!</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hngdcp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1hnexy2</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>Boa Constrictor is the perfect New Years shade 🥰</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0o276icq8e9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1hnel8a</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>I don’t normally go for grays but… 😍</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ylot31p85e9e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1hndpnh</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>Base coats: avoiding staining and peeling?</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hndpnh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1hn43a3</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>In LOVE with Tink’s Wings + recommendation request ✨</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hn43a3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1hn4n51</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>What color should I paint my nails?</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hn4n51/what_color_should_i_paint_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1hn7rfm</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>Christmas nails!</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hn7rfm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1hnch4m</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help! UV top coat is drying without a lamp! </t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hnch4m/help_uv_top_coat_is_drying_without_a_lamp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1hncdlx</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Opi-Kiss me at Midnight </t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/twxa9wx4fd9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1hncbsc</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>Winter nail art</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hncbsc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1hnbujc</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>Littlest laquerista</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hnbujc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1hnblwh</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>I wanna buy from mooncat but for some reason their bottles are exploding?</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hnblwh/i_wanna_buy_from_mooncat_but_for_some_reason/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1hnazvm</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>Winter blues</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hnazvm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1ho0gid</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>Labradorite inspired set on natural nails by @KalsRebelliousNails on IG</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ho0gid</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1hnypic</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>Christmas Nails!!</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hnypic</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1hnwzye</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>New Year’s vibe</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k2wpeay3gi9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1hnvuss</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>Fire Emblem Fates Leo as Stained Glass Painting Nail Art!</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hnvuss</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1hnvu4j</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I made this set, I'm an amateur, what do you think? </t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hnvu4j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1hnvk2b</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>easy nye design ✨️🖤 *contains some gifted pr*</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hnvk2b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1hnuwdl</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>Winter wonderland ❄️🤍</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b18damyvvh9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1hno6fi</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I redid my cake nails! I think this new set came out way better( first pic is old second pic is new) </t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hno6fi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1hnnyk6</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>Tried 2 different colors of cat eye and turned out great 💚</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wmyo7mxs9g9e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1hnm0i3</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I’ve been trying to grow out my nails this year and improve my freehand. Swipe for manis from Jan-Dec! I think it’s slowly getting better! CCW! </t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hnm0i3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1hnlqy8</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Feedback for a newbie / student? </t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hnlqy8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1hnjodd</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>Red and black set</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hnjodd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1hnjc6z</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>🌙✨⭐️Nails</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hnjc6z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1hnisbd</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>A whole entire mood. 🖤</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bguf5xsi5f9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1hnch4w</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t xml:space="preserve">just started and I’m obsessed </t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hnch4w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1hnadb0</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Ocean theme nail art with glowing effect test~</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/p7wky2ldoc9e1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Dec 29 08:09:46 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_12_29.xlsx
+++ b/data/collected_data/2024_12_29.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1204"/>
+  <dimension ref="A1:C1379"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20901,6 +20901,2981 @@
         </is>
       </c>
     </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1hoqzf1</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>First time properly doing Gel X and added regular nail polish on tip</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hoqzf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1hoq7q3</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>Is my manicure putting you in the New Year's mood</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gbhix7gmgq9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1hoq0eg</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First attempt at junk nails </t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hoq0eg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1hop2y8</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>New set 💙</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6nt5i8xw3q9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1hoosu1</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>Christmas nails I did!!!</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hoosu1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1hooda9</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>What can I apply under regular nail polish to prevent nail breakage?</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hooda9/what_can_i_apply_under_regular_nail_polish_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1hoo04f</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>I know absolutely nothing about nails, I don’t take care of them cause I don’t care. I forget they’re even there. So what’s this hard part on the edge of my pinky nail? Have had it before, usually only on the pinky. Solid but a little soft. Usually I just rip it off. What is it?</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hoo04f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1honyhb</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>My Xmas time nails</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1honyhb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1hon6hs</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>Missing Christmas 🎄</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qiyw4ieckp9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1homv14</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t xml:space="preserve">want to start doing my nails -- what shape should I file them to when to grow out? </t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j9hdq4e4hp9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1homs5b</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>I don’t get my nails done, but i was messing with some wax and I see the potential,, is this almond or stiletto lol??</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n88o9oh9gp9e1.gif</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1holxbb</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Winter wonderland nails </t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1holxbb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1hnzl4b</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>Help! What am I missing?</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hnzl4b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1homq4v</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I tried a new base and top coat for gel, and am seeing chipping much earlier than typical. Can I blame the base of the top for this? </t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1homq4v/i_tried_a_new_base_and_top_coat_for_gel_and_am/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1hol0ew</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>how can I fix my vertical ridges?</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hol0ew</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1hom8ha</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>how to stop nails from splitting when they get to a certain length</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hom8ha/how_to_stop_nails_from_splitting_when_they_get_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1hom500</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>I’m obsessed with these nails😍 what do you think?</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hom500</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1hom9hd</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>Unintentionally matched my nails to my wedding ring 😂 nail tech and I love them!</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hom9hd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1hom06q</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>I love how the black color looks on me</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bjjiz8a78p9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1holvqw</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>Obsessed with cat eye</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cv3igyfk7p9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1holtgh</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help me make my new ring pop! </t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/33t0osiy6p9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1holqjz</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Got this idea from a fellow r/nails poster, u/wil8can. My 2024 nail album. </t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1holqjz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1holj91</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First gel set I did myself lasted 3 weeks (&amp; my husband's response) </t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1holj91</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1hokyi9</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>Nail contract</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hokyi9/nail_contract/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1hojaax</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>First manicure- what to ask for?</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hojaax/first_manicure_what_to_ask_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1hokgbu</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>Nail health.</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hokgbu/nail_health/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1hok0wb</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>Coco nails 🤎🤍🤎</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hok0wb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1hoj87y</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>my 21st bday nails</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ngp71rijjo9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1hoil6e</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>My hands are stubby and wrinkly, what nail shape should I get?</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hoil6e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1hoihe8</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>Winter night sky nails</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y3fc95c6do9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1hoih2o</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>New Years Nails</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hoih2o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1hoiac1</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Do you have any feedback? </t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hoiac1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1hoi923</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pink nails </t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kkbtxin6bo9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1hoi7eq</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>Natural nails</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/08vlachsao9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1hoi38g</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>Red line across nails</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0d1xs0es9o9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1hohr70</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time painting my nails in almost a decade. I want to start painting them regularly, but I struggle to keep polish from chipping. </t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z03x10dy6o9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1hohja9</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>Nice tone to close the year...</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hohja9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1hohb3n</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>Just did my nails for New Year’s Day</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hohb3n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1hoh4bl</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>Auditioning looks for NYE</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hoh4bl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1hoh31u</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>Got my Christmas/NY nails in check</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6fdy6pc81o9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1hogt2j</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I told my nail tech to do glitter on glitter with a cat eye and she nailed it 👏 </t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hogt2j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1hoge18</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Natural nail help  </t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hoge18/natural_nail_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1hogdkj</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>Six of my nails broke off to the tip of my finger</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hogdkj/six_of_my_nails_broke_off_to_the_tip_of_my_finger/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1hofum6</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>How do I fix this? I don't want to take them off, but something went wrong and idk why</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/16qq771yqn9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1hog1q9</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>which shape?</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hog1q9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1hog192</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>Question for those of you who wear artificial (glue on) nails</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hog192/question_for_those_of_you_who_wear_artificial/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1hofzfj</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>Was trying to go for a ginger bread house look</t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c008duh3sn9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1hofwxp</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>I painted my nails wanting to have the cat’s eye effect and I think it didn’t work, recommendations?</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hofwxp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1hofvd4</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>Acrylic Overlay or File Down while filling a full set</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hofvd4/acrylic_overlay_or_file_down_while_filling_a_full/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1hofsql</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>New Years Nails 🩷</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6rsanw9jqn9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1hoforb</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>How do I make my Gel X more seamless?</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fc1uq8wlpn9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1hoflsc</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Recent nails </t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hoflsc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1hofi2i</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>Whimsy Lavender Swirls</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9d88id82on9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1hof6z5</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>Baby blue cat eye nails for the New Year 💙</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hof6z5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1hof47f</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>Any BIAB journeys 😊</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hof47f/any_biab_journeys/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1hoet12</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>Feeling Pretty in Pink</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w12qxshdin9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1hoeqin</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>Reddit please help me</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hoeqin/reddit_please_help_me/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1hoeplw</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>Christmas set I did🎄✨</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hoeplw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1hoe2yt</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas nails…. Black with red chrome ombré </t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hoe2yt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1hodwg2</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Glitter me pink!! </t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hodwg2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1hodqw4</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>A classy end to ‘24</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jn3m09lr9n9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1hoar2a</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>Builder Gel Help</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n7ds8j2slm9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1hodacx</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Really proud of how this set turned out. </t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hodacx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1hod1kz</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>Candy cane nails for Christmas!</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gwtqr9s14n9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1hod1g3</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first time getting a builder gel manicure </t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r0dlu9114n9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1hoczi4</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>I wanted a nail that I could wear both at Christmas and New Year's, I love red and glitter, so it turned out like this...</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hoczi4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1hoci2z</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>Types of Nail Glue?</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hoci2z/types_of_nail_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1hocht8</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time doing gel x! </t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mtu80cwozm9e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1hobxlt</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What nail shape looks best? I really dislike my hands. :) </t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hobxlt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1hobf0l</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>glitter for new years!</t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hobf0l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1hobd99</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>Water-ish Nails for my next Cosplay ✨</t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hobd99</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>1hobb60</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t>I can’t decide what to get for my nails next. Any suggestions?</t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hobb60</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>1hoba5w</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>Where are these nail stickers from?</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hoba5w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>1hoapxn</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t>Brand New Wedding Nails</t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d8kk6igilm9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>1ho97mj</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>First time poster seeking improvement tips!</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ho97mj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>1ho1e35</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>After a very disappointing cat eye set, I finally got what I wanted!!</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ho1e35</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>1hoam1z</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Thoughts on press on nails?  </t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hoam1z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>1ho8f39</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Jewel encrusted </t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jfpqdixp2m9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>1ho9glx</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel or acrylic for doing martial arts </t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ho9glx/gel_or_acrylic_for_doing_martial_arts/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>1hoa7xi</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>These are my absolute all time favorite and I've had nails for 5 years!</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0ygw2kmfhm9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>1hoa76z</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t>My New Year's Nails ✨ It's my first time doing hard gel extensions in over 10 years again - I've used solely (gel) nail polish during this time - so I'm a noob, again. Any constructive criticism is appreciated ❤️</t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nwib2nkafm9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>1ho9tfu</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>christmas gifts!</t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/00fiit38em9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>1ho9jyg</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>Need a clear nail strengthener</t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ho9jyg/need_a_clear_nail_strengthener/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>1ho9jho</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First attempt at Chrome ! </t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ho9jho</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>1ho992g</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t>Psychedelic</t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eekmt5kl9m9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1ho932a</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>Super happy with my holiday nails</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a911la478m9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1ho915g</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>New year nail arts with regular polish and some glitter!</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/y86ymabq7m9e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1ho90c0</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>Sparkles for new year's. ✨️</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7t9wel2k7m9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>1ho8nf6</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Has anyone tried the press on nail brand Nailcissist? </t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ho8nf6/has_anyone_tried_the_press_on_nail_brand/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>1ho85m8</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>When your bored at home so apply some fake nails on yourself</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ho85m8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>1ho81hc</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cat eye nails? Have they done them wrong? </t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/061h5wugzl9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>1ho7zad</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>About as long as I've ever gotten them!</t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/68yirj3yyl9e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>1ho7xdl</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fake nail brans </t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ho7xdl/fake_nail_brans/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>1ho7p7d</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Keep practicing </t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ho7p7d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>1ho7m11</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t>Hey, I'm a metalhead (male), I paint sometimes my nails. What do you think ?</t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vvs53j6nvl9e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>1ho77op</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cherry on the top 🍒 </t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/znllpdd3sl9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>1ho6oze</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t>long nails as a cashier</t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sye4n618nl9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>1ho6mp5</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fresh set I love this color </t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fm64xislml9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>1ho3pgd</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t>Can anybody ID color 194?</t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ho3pgd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>1ho4ywy</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t>i have really long nail beds. what shape should i get?</t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sbmn3c165l9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>1hor9eq</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t>What to buy if u want to start doing your own nails with chrome?</t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hor9eq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>1hoqdhj</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t>I have only one question: HOW?! 🤩</t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/o1ifh5soiq9e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>1hoq03v</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Compare ilnp brownstone to holo taco holo cappuccino </t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hoq03v/compare_ilnp_brownstone_to_holo_taco_holo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t>1hopoia</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Some of my Death Valley Nails collection 🏜️ </t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hopoia</t>
+        </is>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr">
+        <is>
+          <t>1hop1kx</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t>December Manis</t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hop1kx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr">
+        <is>
+          <t>1hooxti</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Jelly recs </t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hooxti/jelly_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr">
+        <is>
+          <t>1hoou5a</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t>Aldi nails</t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pxwjx9ob1q9e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="inlineStr">
+        <is>
+          <t>1hoogef</t>
+        </is>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t xml:space="preserve">DVN Glow in the dark </t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hoogef/dvn_glow_in_the_dark/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="inlineStr">
+        <is>
+          <t>1hoofgd</t>
+        </is>
+      </c>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t>What can I apply under regular nail polish to prevent nail breakage? What would be a better choice, acrylic, dip powder, poly gel?</t>
+        </is>
+      </c>
+      <c r="C1313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hoofgd/what_can_i_apply_under_regular_nail_polish_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" t="inlineStr">
+        <is>
+          <t>1honoz3</t>
+        </is>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What indie brands have incredible yellows and oranges? </t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1honoz3/what_indie_brands_have_incredible_yellows_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="inlineStr">
+        <is>
+          <t>1homc41</t>
+        </is>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t>Chamaeleon Nails - Blue Dasher Dragonfly</t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1homc41</t>
+        </is>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" t="inlineStr">
+        <is>
+          <t>1hom9to</t>
+        </is>
+      </c>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t>Bluebird Lacquer "No Egrets"</t>
+        </is>
+      </c>
+      <c r="C1316" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e5bdlgpbbp9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" t="inlineStr">
+        <is>
+          <t>1holz2t</t>
+        </is>
+      </c>
+      <c r="B1317" t="inlineStr">
+        <is>
+          <t>Can’t decide which red(s) to buy!</t>
+        </is>
+      </c>
+      <c r="C1317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1holz2t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" t="inlineStr">
+        <is>
+          <t>1holexl</t>
+        </is>
+      </c>
+      <c r="B1318" t="inlineStr">
+        <is>
+          <t>ILNP Quicksand + Sweet Pea or Sandy Baby?</t>
+        </is>
+      </c>
+      <c r="C1318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1holexl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1319">
+      <c r="A1319" t="inlineStr">
+        <is>
+          <t>1hokvzn</t>
+        </is>
+      </c>
+      <c r="B1319" t="inlineStr">
+        <is>
+          <t>This polish makes me mad</t>
+        </is>
+      </c>
+      <c r="C1319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hokvzn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1320">
+      <c r="A1320" t="inlineStr">
+        <is>
+          <t>1hokvx6</t>
+        </is>
+      </c>
+      <c r="B1320" t="inlineStr">
+        <is>
+          <t>Does anyone here normally have a ‘Model Hand’ with longer nails and a hand with shorter/less pretty nails?</t>
+        </is>
+      </c>
+      <c r="C1320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hokvx6/does_anyone_here_normally_have_a_model_hand_with/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1321">
+      <c r="A1321" t="inlineStr">
+        <is>
+          <t>1hokrhw</t>
+        </is>
+      </c>
+      <c r="B1321" t="inlineStr">
+        <is>
+          <t>Disco ball nails? Don’t mind if I do!!</t>
+        </is>
+      </c>
+      <c r="C1321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hokrhw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" t="inlineStr">
+        <is>
+          <t>1hokkhx</t>
+        </is>
+      </c>
+      <c r="B1322" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Holographic distraction! </t>
+        </is>
+      </c>
+      <c r="C1322" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nd84sa8evo9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1323">
+      <c r="A1323" t="inlineStr">
+        <is>
+          <t>1hokkbo</t>
+        </is>
+      </c>
+      <c r="B1323" t="inlineStr">
+        <is>
+          <t>Ready for New Year's!</t>
+        </is>
+      </c>
+      <c r="C1323" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k7l07vqbvo9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1324">
+      <c r="A1324" t="inlineStr">
+        <is>
+          <t>1hojltn</t>
+        </is>
+      </c>
+      <c r="B1324" t="inlineStr">
+        <is>
+          <t>Mooncat help!</t>
+        </is>
+      </c>
+      <c r="C1324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hojltn/mooncat_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1325">
+      <c r="A1325" t="inlineStr">
+        <is>
+          <t>1hoj08t</t>
+        </is>
+      </c>
+      <c r="B1325" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tried my hand at tortoiseshell nails </t>
+        </is>
+      </c>
+      <c r="C1325" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/83st9luiho9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1326">
+      <c r="A1326" t="inlineStr">
+        <is>
+          <t>1hoihx3</t>
+        </is>
+      </c>
+      <c r="B1326" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Holiday Nails! </t>
+        </is>
+      </c>
+      <c r="C1326" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h4hnomuado9e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1327">
+      <c r="A1327" t="inlineStr">
+        <is>
+          <t>1hoight</t>
+        </is>
+      </c>
+      <c r="B1327" t="inlineStr">
+        <is>
+          <t>Trying to use every polish once</t>
+        </is>
+      </c>
+      <c r="C1327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hoight</t>
+        </is>
+      </c>
+    </row>
+    <row r="1328">
+      <c r="A1328" t="inlineStr">
+        <is>
+          <t>1hoi7su</t>
+        </is>
+      </c>
+      <c r="B1328" t="inlineStr">
+        <is>
+          <t>Does anyone else do a “perpetual manicure?”</t>
+        </is>
+      </c>
+      <c r="C1328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hoi7su/does_anyone_else_do_a_perpetual_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1329">
+      <c r="A1329" t="inlineStr">
+        <is>
+          <t>1hohccs</t>
+        </is>
+      </c>
+      <c r="B1329" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BKL - Luck </t>
+        </is>
+      </c>
+      <c r="C1329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hohccs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1330">
+      <c r="A1330" t="inlineStr">
+        <is>
+          <t>1hohc1l</t>
+        </is>
+      </c>
+      <c r="B1330" t="inlineStr">
+        <is>
+          <t>🌲 Cracked - Tulgey Woods (review) 🌲</t>
+        </is>
+      </c>
+      <c r="C1330" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o1go86ld3o9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1331">
+      <c r="A1331" t="inlineStr">
+        <is>
+          <t>1hogybj</t>
+        </is>
+      </c>
+      <c r="B1331" t="inlineStr">
+        <is>
+          <t>🍕Magentic Pizza🍕</t>
+        </is>
+      </c>
+      <c r="C1331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hogybj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1332">
+      <c r="A1332" t="inlineStr">
+        <is>
+          <t>1hofvg0</t>
+        </is>
+      </c>
+      <c r="B1332" t="inlineStr">
+        <is>
+          <t>(PR) Celestial nails for the fourth night of Hanukkah ✨🌙</t>
+        </is>
+      </c>
+      <c r="C1332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hofvg0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1333">
+      <c r="A1333" t="inlineStr">
+        <is>
+          <t>1hofkbe</t>
+        </is>
+      </c>
+      <c r="B1333" t="inlineStr">
+        <is>
+          <t>First attempt with magnetic</t>
+        </is>
+      </c>
+      <c r="C1333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hofkbe</t>
+        </is>
+      </c>
+    </row>
+    <row r="1334">
+      <c r="A1334" t="inlineStr">
+        <is>
+          <t>1hof7tm</t>
+        </is>
+      </c>
+      <c r="B1334" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Super bling nails! 💎 </t>
+        </is>
+      </c>
+      <c r="C1334" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/n8pey72rln9e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1335">
+      <c r="A1335" t="inlineStr">
+        <is>
+          <t>1hodgok</t>
+        </is>
+      </c>
+      <c r="B1335" t="inlineStr">
+        <is>
+          <t>Holo taco faves</t>
+        </is>
+      </c>
+      <c r="C1335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hodgok/holo_taco_faves/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1336">
+      <c r="A1336" t="inlineStr">
+        <is>
+          <t>1hod7uc</t>
+        </is>
+      </c>
+      <c r="B1336" t="inlineStr">
+        <is>
+          <t>Until I get more storage ... Is it okay if I lay my bottles horizontally like this?</t>
+        </is>
+      </c>
+      <c r="C1336" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/16h1l6fg5n9e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1337">
+      <c r="A1337" t="inlineStr">
+        <is>
+          <t>1hocgvq</t>
+        </is>
+      </c>
+      <c r="B1337" t="inlineStr">
+        <is>
+          <t>nail break + (first) overlay/extension</t>
+        </is>
+      </c>
+      <c r="C1337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hocgvq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1338">
+      <c r="A1338" t="inlineStr">
+        <is>
+          <t>1hoceyc</t>
+        </is>
+      </c>
+      <c r="B1338" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New Year Mani: Cautious Optimism about 2025 </t>
+        </is>
+      </c>
+      <c r="C1338" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ql2elwc1zm9e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1339">
+      <c r="A1339" t="inlineStr">
+        <is>
+          <t>1hob9nw</t>
+        </is>
+      </c>
+      <c r="B1339" t="inlineStr">
+        <is>
+          <t>Nosferatu nails</t>
+        </is>
+      </c>
+      <c r="C1339" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/uimv02svpm9e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1340">
+      <c r="A1340" t="inlineStr">
+        <is>
+          <t>1hob0hv</t>
+        </is>
+      </c>
+      <c r="B1340" t="inlineStr">
+        <is>
+          <t>Perfect Xmas red</t>
+        </is>
+      </c>
+      <c r="C1340" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bpmwg25vnm9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1341">
+      <c r="A1341" t="inlineStr">
+        <is>
+          <t>1hoaukk</t>
+        </is>
+      </c>
+      <c r="B1341" t="inlineStr">
+        <is>
+          <t>NYE skittles!</t>
+        </is>
+      </c>
+      <c r="C1341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hoaukk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1342">
+      <c r="A1342" t="inlineStr">
+        <is>
+          <t>1hoapzv</t>
+        </is>
+      </c>
+      <c r="B1342" t="inlineStr">
+        <is>
+          <t>I finally got my Sassy Sauce order from Black Friday bc Carrie is awesome</t>
+        </is>
+      </c>
+      <c r="C1342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hoapzv/i_finally_got_my_sassy_sauce_order_from_black/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1343">
+      <c r="A1343" t="inlineStr">
+        <is>
+          <t>1hoa296</t>
+        </is>
+      </c>
+      <c r="B1343" t="inlineStr">
+        <is>
+          <t>Does Sassy Sauce offer any kind of shipping discount?</t>
+        </is>
+      </c>
+      <c r="C1343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hoa296/does_sassy_sauce_offer_any_kind_of_shipping/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1344">
+      <c r="A1344" t="inlineStr">
+        <is>
+          <t>1ho9zuj</t>
+        </is>
+      </c>
+      <c r="B1344" t="inlineStr">
+        <is>
+          <t>what is your nail-care routine for ultimate nail health?</t>
+        </is>
+      </c>
+      <c r="C1344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ho9zuj/what_is_your_nailcare_routine_for_ultimate_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1345">
+      <c r="A1345" t="inlineStr">
+        <is>
+          <t>1ho9gf6</t>
+        </is>
+      </c>
+      <c r="B1345" t="inlineStr">
+        <is>
+          <t>Top 5 favourite ILNP polishes</t>
+        </is>
+      </c>
+      <c r="C1345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ho9gf6/top_5_favourite_ilnp_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1346">
+      <c r="A1346" t="inlineStr">
+        <is>
+          <t>1ho6nwk</t>
+        </is>
+      </c>
+      <c r="B1346" t="inlineStr">
+        <is>
+          <t>ILNP Get Cozy</t>
+        </is>
+      </c>
+      <c r="C1346" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3ygikz3uml9e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1347">
+      <c r="A1347" t="inlineStr">
+        <is>
+          <t>1ho6h4c</t>
+        </is>
+      </c>
+      <c r="B1347" t="inlineStr">
+        <is>
+          <t>Fair Isle color?</t>
+        </is>
+      </c>
+      <c r="C1347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ho6h4c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1348">
+      <c r="A1348" t="inlineStr">
+        <is>
+          <t>1ho6gnb</t>
+        </is>
+      </c>
+      <c r="B1348" t="inlineStr">
+        <is>
+          <t>ILNP: Shapeshifter</t>
+        </is>
+      </c>
+      <c r="C1348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ho6gnb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1349">
+      <c r="A1349" t="inlineStr">
+        <is>
+          <t>1ho6a7t</t>
+        </is>
+      </c>
+      <c r="B1349" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Do I have contact dermatitis? </t>
+        </is>
+      </c>
+      <c r="C1349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ho6a7t/do_i_have_contact_dermatitis/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1350">
+      <c r="A1350" t="inlineStr">
+        <is>
+          <t>1ho5bqu</t>
+        </is>
+      </c>
+      <c r="B1350" t="inlineStr">
+        <is>
+          <t>Mid-brightness green shimmer recommendations?</t>
+        </is>
+      </c>
+      <c r="C1350" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/er10le129l9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1351">
+      <c r="A1351" t="inlineStr">
+        <is>
+          <t>1ho59fj</t>
+        </is>
+      </c>
+      <c r="B1351" t="inlineStr">
+        <is>
+          <t>Tell me of beautiful toppers available in the UK!</t>
+        </is>
+      </c>
+      <c r="C1351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ho59fj/tell_me_of_beautiful_toppers_available_in_the_uk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1352">
+      <c r="A1352" t="inlineStr">
+        <is>
+          <t>1ho542p</t>
+        </is>
+      </c>
+      <c r="B1352" t="inlineStr">
+        <is>
+          <t>This light pink pearly polish is beautiful but streaky, bubbly, and doesn't dry hard enough. Can you find a dupe?</t>
+        </is>
+      </c>
+      <c r="C1352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ho542p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1353">
+      <c r="A1353" t="inlineStr">
+        <is>
+          <t>1hnl4z2</t>
+        </is>
+      </c>
+      <c r="B1353" t="inlineStr">
+        <is>
+          <t>I tried doing my own dip powder nails again for the first time in forever!!</t>
+        </is>
+      </c>
+      <c r="C1353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hnl4z2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1354">
+      <c r="A1354" t="inlineStr">
+        <is>
+          <t>1hnpe81</t>
+        </is>
+      </c>
+      <c r="B1354" t="inlineStr">
+        <is>
+          <t>Dupe for “Pound the Pave Mint” by Sally Hansen?</t>
+        </is>
+      </c>
+      <c r="C1354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hnpe81/dupe_for_pound_the_pave_mint_by_sally_hansen/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1355">
+      <c r="A1355" t="inlineStr">
+        <is>
+          <t>1hnsjks</t>
+        </is>
+      </c>
+      <c r="B1355" t="inlineStr">
+        <is>
+          <t>Purple People Eater Vibes</t>
+        </is>
+      </c>
+      <c r="C1355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hnsjks</t>
+        </is>
+      </c>
+    </row>
+    <row r="1356">
+      <c r="A1356" t="inlineStr">
+        <is>
+          <t>1ho3psl</t>
+        </is>
+      </c>
+      <c r="B1356" t="inlineStr">
+        <is>
+          <t>Canmake N101 &amp; N105</t>
+        </is>
+      </c>
+      <c r="C1356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ho3psl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1357">
+      <c r="A1357" t="inlineStr">
+        <is>
+          <t>1ho2le9</t>
+        </is>
+      </c>
+      <c r="B1357" t="inlineStr">
+        <is>
+          <t>Moo Deng</t>
+        </is>
+      </c>
+      <c r="C1357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ho2le9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1358">
+      <c r="A1358" t="inlineStr">
+        <is>
+          <t>1ho1kvd</t>
+        </is>
+      </c>
+      <c r="B1358" t="inlineStr">
+        <is>
+          <t>Painting my way through my Black Friday polishes and obsessed with this color!</t>
+        </is>
+      </c>
+      <c r="C1358" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0ggrabllwj9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1359">
+      <c r="A1359" t="inlineStr">
+        <is>
+          <t>1ho1ex5</t>
+        </is>
+      </c>
+      <c r="B1359" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cracked Polish customer service appreciation post </t>
+        </is>
+      </c>
+      <c r="C1359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ho1ex5/cracked_polish_customer_service_appreciation_post/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1360">
+      <c r="A1360" t="inlineStr">
+        <is>
+          <t>1hor94m</t>
+        </is>
+      </c>
+      <c r="B1360" t="inlineStr">
+        <is>
+          <t>My holiday set ✨️</t>
+        </is>
+      </c>
+      <c r="C1360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dpmd9mestq9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1361">
+      <c r="A1361" t="inlineStr">
+        <is>
+          <t>1hoqi86</t>
+        </is>
+      </c>
+      <c r="B1361" t="inlineStr">
+        <is>
+          <t>The lashes kill meeeee🥲</t>
+        </is>
+      </c>
+      <c r="C1361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hoqi86</t>
+        </is>
+      </c>
+    </row>
+    <row r="1362">
+      <c r="A1362" t="inlineStr">
+        <is>
+          <t>1hoq7ti</t>
+        </is>
+      </c>
+      <c r="B1362" t="inlineStr">
+        <is>
+          <t>Cotton candy chrome 🌌</t>
+        </is>
+      </c>
+      <c r="C1362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hoq7ti</t>
+        </is>
+      </c>
+    </row>
+    <row r="1363">
+      <c r="A1363" t="inlineStr">
+        <is>
+          <t>1hop3g6</t>
+        </is>
+      </c>
+      <c r="B1363" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New set </t>
+        </is>
+      </c>
+      <c r="C1363" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rc4jca524q9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1364">
+      <c r="A1364" t="inlineStr">
+        <is>
+          <t>1hoo8wv</t>
+        </is>
+      </c>
+      <c r="B1364" t="inlineStr">
+        <is>
+          <t>Death Stranding Nails to Satisfy the Gamer in Me (Stamping, Magnetic, Regular Polish)</t>
+        </is>
+      </c>
+      <c r="C1364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hoo8wv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1365">
+      <c r="A1365" t="inlineStr">
+        <is>
+          <t>1honvob</t>
+        </is>
+      </c>
+      <c r="B1365" t="inlineStr">
+        <is>
+          <t>My DiY nails (Nail wraps)</t>
+        </is>
+      </c>
+      <c r="C1365" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kigqtd0frp9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1366">
+      <c r="A1366" t="inlineStr">
+        <is>
+          <t>1honsbq</t>
+        </is>
+      </c>
+      <c r="B1366" t="inlineStr">
+        <is>
+          <t>Dragon inspired</t>
+        </is>
+      </c>
+      <c r="C1366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1honsbq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1367">
+      <c r="A1367" t="inlineStr">
+        <is>
+          <t>1hokay0</t>
+        </is>
+      </c>
+      <c r="B1367" t="inlineStr">
+        <is>
+          <t>Todays order ✨</t>
+        </is>
+      </c>
+      <c r="C1367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hokay0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1368">
+      <c r="A1368" t="inlineStr">
+        <is>
+          <t>1hohha4</t>
+        </is>
+      </c>
+      <c r="B1368" t="inlineStr">
+        <is>
+          <t>New Year, New Nails</t>
+        </is>
+      </c>
+      <c r="C1368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hohha4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1369">
+      <c r="A1369" t="inlineStr">
+        <is>
+          <t>1hogqmy</t>
+        </is>
+      </c>
+      <c r="B1369" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Last minute Xmas nails </t>
+        </is>
+      </c>
+      <c r="C1369" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/16tj84zdyn9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1370">
+      <c r="A1370" t="inlineStr">
+        <is>
+          <t>1hoezq1</t>
+        </is>
+      </c>
+      <c r="B1370" t="inlineStr">
+        <is>
+          <t>Mixed metals</t>
+        </is>
+      </c>
+      <c r="C1370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hoezq1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1371">
+      <c r="A1371" t="inlineStr">
+        <is>
+          <t>1hobyms</t>
+        </is>
+      </c>
+      <c r="B1371" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I’m not ready to say goodbye. 3 weeks of grow out 💅🏼 </t>
+        </is>
+      </c>
+      <c r="C1371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hobyms</t>
+        </is>
+      </c>
+    </row>
+    <row r="1372">
+      <c r="A1372" t="inlineStr">
+        <is>
+          <t>1hob67h</t>
+        </is>
+      </c>
+      <c r="B1372" t="inlineStr">
+        <is>
+          <t>Red and Gold Sparkle</t>
+        </is>
+      </c>
+      <c r="C1372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hob67h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1373">
+      <c r="A1373" t="inlineStr">
+        <is>
+          <t>1hoaqwj</t>
+        </is>
+      </c>
+      <c r="B1373" t="inlineStr">
+        <is>
+          <t>New Years Nails 🩷</t>
+        </is>
+      </c>
+      <c r="C1373" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z5sbikpqlm9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1374">
+      <c r="A1374" t="inlineStr">
+        <is>
+          <t>1ho9o1t</t>
+        </is>
+      </c>
+      <c r="B1374" t="inlineStr">
+        <is>
+          <t>16 and been doing nails for abt a year. Be honest, any advice is welcome :)</t>
+        </is>
+      </c>
+      <c r="C1374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ho9o1t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1375">
+      <c r="A1375" t="inlineStr">
+        <is>
+          <t>1ho968o</t>
+        </is>
+      </c>
+      <c r="B1375" t="inlineStr">
+        <is>
+          <t>New year nail arts with regular polish and some glitter!</t>
+        </is>
+      </c>
+      <c r="C1375" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9i5chttw8m9e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1376">
+      <c r="A1376" t="inlineStr">
+        <is>
+          <t>1ho8qh6</t>
+        </is>
+      </c>
+      <c r="B1376" t="inlineStr">
+        <is>
+          <t>Cute christmas tree nails</t>
+        </is>
+      </c>
+      <c r="C1376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ho8qh6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1377">
+      <c r="A1377" t="inlineStr">
+        <is>
+          <t>1ho84w2</t>
+        </is>
+      </c>
+      <c r="B1377" t="inlineStr">
+        <is>
+          <t>Jewel encrusted</t>
+        </is>
+      </c>
+      <c r="C1377" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zpqz1y5a0m9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1378">
+      <c r="A1378" t="inlineStr">
+        <is>
+          <t>1ho6nrf</t>
+        </is>
+      </c>
+      <c r="B1378" t="inlineStr">
+        <is>
+          <t>I tried to do delicate flowers on nails!</t>
+        </is>
+      </c>
+      <c r="C1378" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=VFzqK7XYaY8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1379">
+      <c r="A1379" t="inlineStr">
+        <is>
+          <t>1ho1v1n</t>
+        </is>
+      </c>
+      <c r="B1379" t="inlineStr">
+        <is>
+          <t>New year nails 2025 💕</t>
+        </is>
+      </c>
+      <c r="C1379" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sgthkonj0k9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>